<commit_message>
finished IRR round 1 for final feature extraction
</commit_message>
<xml_diff>
--- a/S18_Environment_Feature_Extraction.xlsx
+++ b/S18_Environment_Feature_Extraction.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3411" uniqueCount="695">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3502" uniqueCount="712">
   <si>
     <t>UUID</t>
   </si>
@@ -2159,10 +2159,10 @@
     <t>individual, multi-person, both, unspecified</t>
   </si>
   <si>
-    <t>instructional, training, informal</t>
-  </si>
-  <si>
-    <t>K-12, undergraduate, graduate, professional development, undisclosed</t>
+    <t>instructional, training, informal, unspecified</t>
+  </si>
+  <si>
+    <t>K-12, undergraduate, graduate, professional development, unspecified</t>
   </si>
   <si>
     <t>model-based, model-free</t>
@@ -2230,6 +2230,62 @@
   </si>
   <si>
     <t>Orchestration graphs. Multi-person because classroom-based and therefore multiple students.</t>
+  </si>
+  <si>
+    <t>Marvy learns (geometry). RF for classification (model-based). Exploratory Factor Analysis (EFA) for statistical analysis (model-free)</t>
+  </si>
+  <si>
+    <t>informal</t>
+  </si>
+  <si>
+    <t>professional</t>
+  </si>
+  <si>
+    <t>"We conducted a case study to compare the visualizations provided by the system in two different situations: collaborative and competitive activities. The results suggest that the provided visualizations help to identify issues on cognitive contribution, assimilation, self-regulation, and integration of the team members. They could also support teachers to decide whether they must assist a team in fostering collaboration.
+While the results are naturally constrained to the characteristics of the activities in which we tested the platform, they provide initial evidence about the technical fea-
+sibility of extracting behavioral indicators and traces using MMLA to give insights onteam collaboration."</t>
+  </si>
+  <si>
+    <t>undergraduate</t>
+  </si>
+  <si>
+    <t>Arduino + browser IDE, so blended engineering. DNN + regression. Also tested SVM, NB, LR.</t>
+  </si>
+  <si>
+    <t>2 tasks: use sheet of paper to hold text book, and use other materials to support a 0.5lb mass
+Model-based w/ DT classifier, model-free with k-means clustering.</t>
+  </si>
+  <si>
+    <t>Table Tennis Tutor, LSTM classification.</t>
+  </si>
+  <si>
+    <t>"Overall, our work shows that capturing multimodal data can help us increase the prediction accuracy of users’ learning performance in learner–computer interaction (LCI). In addition, the study shows that the most commonly used data-stream (i.e., keystrokes) is the poorest proxy of our learning performance. Thus, leveraging advances in contemporary learning environments and physiological sensing (wearable, EEG etc.), we provide evidence that multimodal data can be a viable method to accurately track users’ states during learning, thereby providing unique possibilities of closing the loop between the learning technology and the learner. Therefore, the incorporation of multimodal data enables HCI and learning technology researchers to examine unscripted, complex tasks in more holistic and accurate ways."
+Identified specific multimodal features that were best predictors of performance.</t>
+  </si>
+  <si>
+    <t>Pac-Man. Model-based for regression, model-free for statistical methods.
+Does training always map to training or is Pacman both a training environment that is informal, for instance?</t>
+  </si>
+  <si>
+    <t>Engagement detection, DAiSEE dataset. Neural Turing Machine (NTM) RNN.</t>
+  </si>
+  <si>
+    <t>Affect detection in simulated medical environment. "other" for environment type because medical? SVM and DNN for model-based.</t>
+  </si>
+  <si>
+    <t>virtual, physical</t>
+  </si>
+  <si>
+    <t>individual, multi-student</t>
+  </si>
+  <si>
+    <t>Ashwin paper! Automated inquiry-based instruction based on affective state. Two environments: classroom (multi-student) and e-learning (single-student). Classification via Inception and YOLO.</t>
+  </si>
+  <si>
+    <t>Learning CS w/ Snap! collaboratively. SVM, BERT, MLP for model-based.</t>
+  </si>
+  <si>
+    <t>Monash nursing group. Other for healthcare?</t>
   </si>
 </sst>
 </file>
@@ -2260,7 +2316,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2289,6 +2345,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB6D7A8"/>
         <bgColor rgb="FFB6D7A8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFF0000"/>
       </patternFill>
     </fill>
   </fills>
@@ -2364,6 +2426,9 @@
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
@@ -2371,9 +2436,6 @@
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
@@ -2384,7 +2446,7 @@
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2732,7 +2794,7 @@
       <c r="AA2" s="7"/>
       <c r="AB2" s="7"/>
     </row>
-    <row r="3" hidden="1">
+    <row r="3">
       <c r="A3" s="8">
         <v>1.326191931E9</v>
       </c>
@@ -2791,7 +2853,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="4" hidden="1">
+    <row r="4">
       <c r="A4" s="8">
         <v>1.326191931E9</v>
       </c>
@@ -2840,7 +2902,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="5" hidden="1">
+    <row r="5">
       <c r="A5" s="8">
         <v>1.469065963E9</v>
       </c>
@@ -2899,7 +2961,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="6" hidden="1">
+    <row r="6">
       <c r="A6" s="8">
         <v>1.469065963E9</v>
       </c>
@@ -2948,7 +3010,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="7" hidden="1">
+    <row r="7">
       <c r="A7" s="8">
         <v>1.598166515E9</v>
       </c>
@@ -3007,7 +3069,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="8" hidden="1">
+    <row r="8">
       <c r="A8" s="8">
         <v>1.598166515E9</v>
       </c>
@@ -3056,7 +3118,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="9" hidden="1">
+    <row r="9">
       <c r="A9" s="8">
         <v>1.877483551E9</v>
       </c>
@@ -3115,7 +3177,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="10" hidden="1">
+    <row r="10">
       <c r="A10" s="8">
         <v>1.877483551E9</v>
       </c>
@@ -3164,7 +3226,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="11" hidden="1">
+    <row r="11">
       <c r="A11" s="8">
         <v>2.000036002E9</v>
       </c>
@@ -3223,7 +3285,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="12" hidden="1">
+    <row r="12">
       <c r="A12" s="8">
         <v>2.000036002E9</v>
       </c>
@@ -3272,7 +3334,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="13" hidden="1">
+    <row r="13">
       <c r="A13" s="8">
         <v>2.070224207E9</v>
       </c>
@@ -3331,7 +3393,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="14" hidden="1">
+    <row r="14">
       <c r="A14" s="8">
         <v>2.070224207E9</v>
       </c>
@@ -3380,7 +3442,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="15" hidden="1">
+    <row r="15">
       <c r="A15" s="8">
         <v>2.634033325E9</v>
       </c>
@@ -3439,7 +3501,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="16" hidden="1">
+    <row r="16">
       <c r="A16" s="8">
         <v>2.634033325E9</v>
       </c>
@@ -3488,7 +3550,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="17" hidden="1">
+    <row r="17">
       <c r="A17" s="8">
         <v>3.051560548E9</v>
       </c>
@@ -3547,7 +3609,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="18" hidden="1">
+    <row r="18">
       <c r="A18" s="8">
         <v>3.051560548E9</v>
       </c>
@@ -3596,7 +3658,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="19" hidden="1">
+    <row r="19">
       <c r="A19" s="8">
         <v>3.339002981E9</v>
       </c>
@@ -3655,7 +3717,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="20" hidden="1">
+    <row r="20">
       <c r="A20" s="8">
         <v>3.339002981E9</v>
       </c>
@@ -3704,7 +3766,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="21" hidden="1">
+    <row r="21">
       <c r="A21" s="8">
         <v>3.408664396E9</v>
       </c>
@@ -3761,7 +3823,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="22" ht="15.75" hidden="1" customHeight="1">
+    <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="8">
         <v>3.408664396E9</v>
       </c>
@@ -3810,7 +3872,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="23" ht="15.75" hidden="1" customHeight="1">
+    <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="8">
         <v>8.04659204E8</v>
       </c>
@@ -3869,7 +3931,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="24" ht="15.75" hidden="1" customHeight="1">
+    <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="8">
         <v>8.04659204E8</v>
       </c>
@@ -3918,7 +3980,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="25" ht="15.75" hidden="1" customHeight="1">
+    <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="8">
         <v>1.581261659E9</v>
       </c>
@@ -3977,7 +4039,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="26" ht="15.75" hidden="1" customHeight="1">
+    <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="8">
         <v>1.581261659E9</v>
       </c>
@@ -4026,7 +4088,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="27" ht="15.75" hidden="1" customHeight="1">
+    <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="8">
         <v>2.836996318E9</v>
       </c>
@@ -4085,7 +4147,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="28" ht="15.75" hidden="1" customHeight="1">
+    <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="8">
         <v>2.836996318E9</v>
       </c>
@@ -4134,7 +4196,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="29" ht="15.75" hidden="1" customHeight="1">
+    <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="8">
         <v>3.2184286E7</v>
       </c>
@@ -4193,7 +4255,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="30" ht="15.75" hidden="1" customHeight="1">
+    <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="8">
         <v>3.2184286E7</v>
       </c>
@@ -4242,7 +4304,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="31" ht="15.75" hidden="1" customHeight="1">
+    <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="8">
         <v>4.33919853E8</v>
       </c>
@@ -4301,7 +4363,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="32" ht="15.75" hidden="1" customHeight="1">
+    <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="8">
         <v>4.33919853E8</v>
       </c>
@@ -4350,7 +4412,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="33" ht="15.75" hidden="1" customHeight="1">
+    <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="8">
         <v>4.83140962E8</v>
       </c>
@@ -4409,7 +4471,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="34" ht="15.75" hidden="1" customHeight="1">
+    <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="8">
         <v>4.83140962E8</v>
       </c>
@@ -4458,7 +4520,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="35" ht="15.75" hidden="1" customHeight="1">
+    <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="8">
         <v>3.308658121E9</v>
       </c>
@@ -4517,7 +4579,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="36" ht="15.75" hidden="1" customHeight="1">
+    <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="8">
         <v>3.308658121E9</v>
       </c>
@@ -4566,7 +4628,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="37" ht="15.75" hidden="1" customHeight="1">
+    <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="8">
         <v>1.847468084E9</v>
       </c>
@@ -4625,7 +4687,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="38" ht="15.75" hidden="1" customHeight="1">
+    <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="8">
         <v>1.847468084E9</v>
       </c>
@@ -4674,7 +4736,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="39" ht="15.75" hidden="1" customHeight="1">
+    <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="8">
         <v>2.345021698E9</v>
       </c>
@@ -4733,7 +4795,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="40" ht="15.75" hidden="1" customHeight="1">
+    <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="8">
         <v>2.345021698E9</v>
       </c>
@@ -4782,7 +4844,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="41" ht="15.75" hidden="1" customHeight="1">
+    <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="8">
         <v>3.796643912E9</v>
       </c>
@@ -4844,7 +4906,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="42" ht="15.75" hidden="1" customHeight="1">
+    <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="8">
         <v>3.796643912E9</v>
       </c>
@@ -4893,7 +4955,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="43" ht="15.75" hidden="1" customHeight="1">
+    <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="8">
         <v>2.05660768E8</v>
       </c>
@@ -4952,7 +5014,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="44" ht="15.75" hidden="1" customHeight="1">
+    <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="8">
         <v>2.05660768E8</v>
       </c>
@@ -5001,7 +5063,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="45" ht="15.75" hidden="1" customHeight="1">
+    <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="8">
         <v>2.18163761E9</v>
       </c>
@@ -5060,7 +5122,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="46" ht="15.75" hidden="1" customHeight="1">
+    <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="8">
         <v>2.18163761E9</v>
       </c>
@@ -5109,7 +5171,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="47" ht="15.75" hidden="1" customHeight="1">
+    <row r="47" ht="15.75" customHeight="1">
       <c r="A47" s="8">
         <v>4.035649049E9</v>
       </c>
@@ -5168,7 +5230,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="48" ht="15.75" hidden="1" customHeight="1">
+    <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="8">
         <v>4.035649049E9</v>
       </c>
@@ -5217,7 +5279,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="49" ht="15.75" hidden="1" customHeight="1">
+    <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="8">
         <v>1.019093033E9</v>
       </c>
@@ -5276,7 +5338,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="50" ht="15.75" hidden="1" customHeight="1">
+    <row r="50" ht="15.75" customHeight="1">
       <c r="A50" s="8">
         <v>1.019093033E9</v>
       </c>
@@ -5325,7 +5387,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="51" ht="15.75" hidden="1" customHeight="1">
+    <row r="51" ht="15.75" customHeight="1">
       <c r="A51" s="8">
         <v>2.936220551E9</v>
       </c>
@@ -5384,7 +5446,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="52" ht="15.75" hidden="1" customHeight="1">
+    <row r="52" ht="15.75" customHeight="1">
       <c r="A52" s="8">
         <v>2.936220551E9</v>
       </c>
@@ -5433,7 +5495,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="53" ht="15.75" hidden="1" customHeight="1">
+    <row r="53" ht="15.75" customHeight="1">
       <c r="A53" s="8">
         <v>1.886134458E9</v>
       </c>
@@ -5492,7 +5554,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="54" ht="15.75" hidden="1" customHeight="1">
+    <row r="54" ht="15.75" customHeight="1">
       <c r="A54" s="8">
         <v>1.886134458E9</v>
       </c>
@@ -5541,7 +5603,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="55" ht="15.75" hidden="1" customHeight="1">
+    <row r="55" ht="15.75" customHeight="1">
       <c r="A55" s="8">
         <v>2.879332689E9</v>
       </c>
@@ -5600,7 +5662,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="56" ht="15.75" hidden="1" customHeight="1">
+    <row r="56" ht="15.75" customHeight="1">
       <c r="A56" s="8">
         <v>2.879332689E9</v>
       </c>
@@ -5649,7 +5711,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="57" ht="15.75" hidden="1" customHeight="1">
+    <row r="57" ht="15.75" customHeight="1">
       <c r="A57" s="8">
         <v>3.146393211E9</v>
       </c>
@@ -5708,7 +5770,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="58" ht="15.75" hidden="1" customHeight="1">
+    <row r="58" ht="15.75" customHeight="1">
       <c r="A58" s="8">
         <v>3.146393211E9</v>
       </c>
@@ -5757,7 +5819,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="59" ht="15.75" hidden="1" customHeight="1">
+    <row r="59" ht="15.75" customHeight="1">
       <c r="A59" s="8">
         <v>3.809293172E9</v>
       </c>
@@ -5816,7 +5878,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="60" ht="15.75" hidden="1" customHeight="1">
+    <row r="60" ht="15.75" customHeight="1">
       <c r="A60" s="8">
         <v>3.809293172E9</v>
       </c>
@@ -5865,7 +5927,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="61" ht="15.75" hidden="1" customHeight="1">
+    <row r="61" ht="15.75" customHeight="1">
       <c r="A61" s="8">
         <v>4.019205162E9</v>
       </c>
@@ -5924,7 +5986,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="62" ht="15.75" hidden="1" customHeight="1">
+    <row r="62" ht="15.75" customHeight="1">
       <c r="A62" s="8">
         <v>4.019205162E9</v>
       </c>
@@ -5973,7 +6035,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="63" ht="15.75" hidden="1" customHeight="1">
+    <row r="63" ht="15.75" customHeight="1">
       <c r="A63" s="8">
         <v>4.27781205E9</v>
       </c>
@@ -6032,7 +6094,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="64" ht="15.75" hidden="1" customHeight="1">
+    <row r="64" ht="15.75" customHeight="1">
       <c r="A64" s="8">
         <v>4.27781205E9</v>
       </c>
@@ -6081,7 +6143,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="65" ht="15.75" hidden="1" customHeight="1">
+    <row r="65" ht="15.75" customHeight="1">
       <c r="A65" s="8">
         <v>1.609706685E9</v>
       </c>
@@ -6140,7 +6202,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="66" ht="15.75" hidden="1" customHeight="1">
+    <row r="66" ht="15.75" customHeight="1">
       <c r="A66" s="8">
         <v>1.609706685E9</v>
       </c>
@@ -6189,7 +6251,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="67" ht="15.75" hidden="1" customHeight="1">
+    <row r="67" ht="15.75" customHeight="1">
       <c r="A67" s="8">
         <v>3.398902089E9</v>
       </c>
@@ -6248,7 +6310,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="68" ht="15.75" hidden="1" customHeight="1">
+    <row r="68" ht="15.75" customHeight="1">
       <c r="A68" s="8">
         <v>3.398902089E9</v>
       </c>
@@ -6297,7 +6359,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="69" ht="15.75" hidden="1" customHeight="1">
+    <row r="69" ht="15.75" customHeight="1">
       <c r="A69" s="8">
         <v>3.093310941E9</v>
       </c>
@@ -6356,7 +6418,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="70" ht="15.75" hidden="1" customHeight="1">
+    <row r="70" ht="15.75" customHeight="1">
       <c r="A70" s="8">
         <v>3.093310941E9</v>
       </c>
@@ -6405,7 +6467,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="71" ht="15.75" hidden="1" customHeight="1">
+    <row r="71" ht="15.75" customHeight="1">
       <c r="A71" s="8">
         <v>1.576545447E9</v>
       </c>
@@ -6464,7 +6526,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="72" ht="15.75" hidden="1" customHeight="1">
+    <row r="72" ht="15.75" customHeight="1">
       <c r="A72" s="8">
         <v>1.576545447E9</v>
       </c>
@@ -6513,7 +6575,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="73" ht="15.75" hidden="1" customHeight="1">
+    <row r="73" ht="15.75" customHeight="1">
       <c r="A73" s="8">
         <v>3.796180663E9</v>
       </c>
@@ -6572,7 +6634,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="74" ht="15.75" hidden="1" customHeight="1">
+    <row r="74" ht="15.75" customHeight="1">
       <c r="A74" s="8">
         <v>3.796180663E9</v>
       </c>
@@ -6621,7 +6683,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="75" ht="15.75" hidden="1" customHeight="1">
+    <row r="75" ht="15.75" customHeight="1">
       <c r="A75" s="8">
         <v>1.770989706E9</v>
       </c>
@@ -6680,7 +6742,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="76" ht="15.75" hidden="1" customHeight="1">
+    <row r="76" ht="15.75" customHeight="1">
       <c r="A76" s="8">
         <v>1.770989706E9</v>
       </c>
@@ -6729,7 +6791,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="77" ht="15.75" hidden="1" customHeight="1">
+    <row r="77" ht="15.75" customHeight="1">
       <c r="A77" s="8">
         <v>2.456887548E9</v>
       </c>
@@ -6788,7 +6850,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="78" ht="15.75" hidden="1" customHeight="1">
+    <row r="78" ht="15.75" customHeight="1">
       <c r="A78" s="8">
         <v>2.456887548E9</v>
       </c>
@@ -6837,7 +6899,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="79" ht="15.75" hidden="1" customHeight="1">
+    <row r="79" ht="15.75" customHeight="1">
       <c r="A79" s="8">
         <v>5.18268671E8</v>
       </c>
@@ -6896,7 +6958,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="80" ht="15.75" hidden="1" customHeight="1">
+    <row r="80" ht="15.75" customHeight="1">
       <c r="A80" s="8">
         <v>5.18268671E8</v>
       </c>
@@ -6945,7 +7007,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="81" ht="15.75" hidden="1" customHeight="1">
+    <row r="81" ht="15.75" customHeight="1">
       <c r="A81" s="8">
         <v>9.57160695E8</v>
       </c>
@@ -7004,7 +7066,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="82" ht="15.75" hidden="1" customHeight="1">
+    <row r="82" ht="15.75" customHeight="1">
       <c r="A82" s="8">
         <v>9.57160695E8</v>
       </c>
@@ -7053,7 +7115,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="83" ht="15.75" hidden="1" customHeight="1">
+    <row r="83" ht="15.75" customHeight="1">
       <c r="A83" s="8">
         <v>3.00954867E9</v>
       </c>
@@ -7112,7 +7174,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="84" ht="15.75" hidden="1" customHeight="1">
+    <row r="84" ht="15.75" customHeight="1">
       <c r="A84" s="8">
         <v>3.00954867E9</v>
       </c>
@@ -7161,7 +7223,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="85" ht="15.75" hidden="1" customHeight="1">
+    <row r="85" ht="15.75" customHeight="1">
       <c r="A85" s="8">
         <v>3.448122334E9</v>
       </c>
@@ -7220,7 +7282,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="86" ht="15.75" hidden="1" customHeight="1">
+    <row r="86" ht="15.75" customHeight="1">
       <c r="A86" s="8">
         <v>3.448122334E9</v>
       </c>
@@ -7269,7 +7331,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="87" ht="15.75" hidden="1" customHeight="1">
+    <row r="87" ht="15.75" customHeight="1">
       <c r="A87" s="8">
         <v>2.497456347E9</v>
       </c>
@@ -7328,7 +7390,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="88" ht="15.75" hidden="1" customHeight="1">
+    <row r="88" ht="15.75" customHeight="1">
       <c r="A88" s="8">
         <v>2.497456347E9</v>
       </c>
@@ -7377,7 +7439,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="89" ht="15.75" hidden="1" customHeight="1">
+    <row r="89" ht="15.75" customHeight="1">
       <c r="A89" s="8">
         <v>3.660066725E9</v>
       </c>
@@ -7436,7 +7498,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="90" ht="15.75" hidden="1" customHeight="1">
+    <row r="90" ht="15.75" customHeight="1">
       <c r="A90" s="8">
         <v>3.660066725E9</v>
       </c>
@@ -7485,7 +7547,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="91" ht="15.75" hidden="1" customHeight="1">
+    <row r="91" ht="15.75" customHeight="1">
       <c r="A91" s="8">
         <v>3.783339081E9</v>
       </c>
@@ -7544,7 +7606,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="92" ht="15.75" hidden="1" customHeight="1">
+    <row r="92" ht="15.75" customHeight="1">
       <c r="A92" s="8">
         <v>3.783339081E9</v>
       </c>
@@ -7593,7 +7655,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="93" ht="15.75" hidden="1" customHeight="1">
+    <row r="93" ht="15.75" customHeight="1">
       <c r="A93" s="8">
         <v>3.095923626E9</v>
       </c>
@@ -7652,7 +7714,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="94" ht="15.75" hidden="1" customHeight="1">
+    <row r="94" ht="15.75" customHeight="1">
       <c r="A94" s="8">
         <v>3.095923626E9</v>
       </c>
@@ -7701,7 +7763,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="95" ht="15.75" hidden="1" customHeight="1">
+    <row r="95" ht="15.75" customHeight="1">
       <c r="A95" s="8">
         <v>8.5990093E7</v>
       </c>
@@ -7760,7 +7822,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="96" ht="15.75" hidden="1" customHeight="1">
+    <row r="96" ht="15.75" customHeight="1">
       <c r="A96" s="8">
         <v>8.5990093E7</v>
       </c>
@@ -7809,7 +7871,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="97" ht="15.75" hidden="1" customHeight="1">
+    <row r="97" ht="15.75" customHeight="1">
       <c r="A97" s="8">
         <v>8.6191824E7</v>
       </c>
@@ -7868,7 +7930,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="98" ht="15.75" hidden="1" customHeight="1">
+    <row r="98" ht="15.75" customHeight="1">
       <c r="A98" s="8">
         <v>8.6191824E7</v>
       </c>
@@ -7917,7 +7979,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="99" ht="15.75" hidden="1" customHeight="1">
+    <row r="99" ht="15.75" customHeight="1">
       <c r="A99" s="8">
         <v>8.18492192E8</v>
       </c>
@@ -7976,7 +8038,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="100" ht="15.75" hidden="1" customHeight="1">
+    <row r="100" ht="15.75" customHeight="1">
       <c r="A100" s="8">
         <v>8.18492192E8</v>
       </c>
@@ -8025,7 +8087,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="101" ht="15.75" hidden="1" customHeight="1">
+    <row r="101" ht="15.75" customHeight="1">
       <c r="A101" s="8">
         <v>1.47203129E8</v>
       </c>
@@ -8084,7 +8146,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="102" ht="15.75" hidden="1" customHeight="1">
+    <row r="102" ht="15.75" customHeight="1">
       <c r="A102" s="8">
         <v>1.47203129E8</v>
       </c>
@@ -8133,7 +8195,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="103" ht="15.75" hidden="1" customHeight="1">
+    <row r="103" ht="15.75" customHeight="1">
       <c r="A103" s="8">
         <v>1.23412197E8</v>
       </c>
@@ -8192,7 +8254,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="104" ht="15.75" hidden="1" customHeight="1">
+    <row r="104" ht="15.75" customHeight="1">
       <c r="A104" s="8">
         <v>1.23412197E8</v>
       </c>
@@ -8241,7 +8303,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="105" ht="15.75" hidden="1" customHeight="1">
+    <row r="105" ht="15.75" customHeight="1">
       <c r="A105" s="8">
         <v>1.118315889E9</v>
       </c>
@@ -8300,7 +8362,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="106" ht="15.75" hidden="1" customHeight="1">
+    <row r="106" ht="15.75" customHeight="1">
       <c r="A106" s="8">
         <v>1.118315889E9</v>
       </c>
@@ -8349,7 +8411,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="107" ht="15.75" hidden="1" customHeight="1">
+    <row r="107" ht="15.75" customHeight="1">
       <c r="A107" s="8">
         <v>1.315379489E9</v>
       </c>
@@ -8408,7 +8470,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="108" ht="15.75" hidden="1" customHeight="1">
+    <row r="108" ht="15.75" customHeight="1">
       <c r="A108" s="8">
         <v>1.315379489E9</v>
       </c>
@@ -8457,7 +8519,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="109" ht="15.75" hidden="1" customHeight="1">
+    <row r="109" ht="15.75" customHeight="1">
       <c r="A109" s="8">
         <v>1.374035721E9</v>
       </c>
@@ -8516,7 +8578,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="110" ht="15.75" hidden="1" customHeight="1">
+    <row r="110" ht="15.75" customHeight="1">
       <c r="A110" s="8">
         <v>1.374035721E9</v>
       </c>
@@ -8565,7 +8627,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="111" ht="15.75" hidden="1" customHeight="1">
+    <row r="111" ht="15.75" customHeight="1">
       <c r="A111" s="8">
         <v>1.426267857E9</v>
       </c>
@@ -8624,7 +8686,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="112" ht="15.75" hidden="1" customHeight="1">
+    <row r="112" ht="15.75" customHeight="1">
       <c r="A112" s="8">
         <v>1.426267857E9</v>
       </c>
@@ -8743,7 +8805,7 @@
       <c r="AA113" s="18"/>
       <c r="AB113" s="18"/>
     </row>
-    <row r="114" ht="15.75" hidden="1" customHeight="1">
+    <row r="114" ht="15.75" customHeight="1">
       <c r="A114" s="8">
         <v>2.055153191E9</v>
       </c>
@@ -8862,7 +8924,7 @@
       <c r="AA115" s="18"/>
       <c r="AB115" s="18"/>
     </row>
-    <row r="116" ht="15.75" hidden="1" customHeight="1">
+    <row r="116" ht="15.75" customHeight="1">
       <c r="A116" s="8">
         <v>2.273914836E9</v>
       </c>
@@ -8981,7 +9043,7 @@
       <c r="AA117" s="18"/>
       <c r="AB117" s="18"/>
     </row>
-    <row r="118" ht="15.75" hidden="1" customHeight="1">
+    <row r="118" ht="15.75" customHeight="1">
       <c r="A118" s="8">
         <v>1.763513559E9</v>
       </c>
@@ -9100,7 +9162,7 @@
       <c r="AA119" s="18"/>
       <c r="AB119" s="18"/>
     </row>
-    <row r="120" ht="15.75" hidden="1" customHeight="1">
+    <row r="120" ht="15.75" customHeight="1">
       <c r="A120" s="8">
         <v>1.345598079E9</v>
       </c>
@@ -9219,7 +9281,7 @@
       <c r="AA121" s="18"/>
       <c r="AB121" s="18"/>
     </row>
-    <row r="122" ht="15.75" hidden="1" customHeight="1">
+    <row r="122" ht="15.75" customHeight="1">
       <c r="A122" s="8">
         <v>3.135645357E9</v>
       </c>
@@ -9269,76 +9331,76 @@
       </c>
     </row>
     <row r="123" ht="15.75" customHeight="1">
-      <c r="A123" s="19">
+      <c r="A123" s="16">
         <v>3.856280479E9</v>
       </c>
-      <c r="B123" s="19" t="s">
+      <c r="B123" s="16" t="s">
         <v>548</v>
       </c>
-      <c r="C123" s="19" t="s">
+      <c r="C123" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="D123" s="19">
+      <c r="D123" s="16">
         <v>2021.0</v>
       </c>
-      <c r="E123" s="19" t="s">
+      <c r="E123" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="F123" s="19" t="s">
+      <c r="F123" s="16" t="s">
         <v>412</v>
       </c>
-      <c r="G123" s="19" t="s">
+      <c r="G123" s="16" t="s">
         <v>549</v>
       </c>
-      <c r="H123" s="19" t="s">
+      <c r="H123" s="16" t="s">
         <v>550</v>
       </c>
-      <c r="I123" s="19" t="s">
+      <c r="I123" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="J123" s="19" t="s">
+      <c r="J123" s="16" t="s">
         <v>290</v>
       </c>
-      <c r="K123" s="19" t="s">
+      <c r="K123" s="16" t="s">
         <v>291</v>
       </c>
-      <c r="L123" s="19">
+      <c r="L123" s="16">
         <v>35.0</v>
       </c>
-      <c r="M123" s="20" t="s">
+      <c r="M123" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="N123" s="20" t="s">
+      <c r="N123" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="O123" s="20" t="s">
+      <c r="O123" s="17" t="s">
         <v>551</v>
       </c>
-      <c r="P123" s="20" t="s">
+      <c r="P123" s="17" t="s">
         <v>552</v>
       </c>
-      <c r="Q123" s="20" t="s">
+      <c r="Q123" s="17" t="s">
         <v>553</v>
       </c>
-      <c r="R123" s="19" t="s">
+      <c r="R123" s="16" t="s">
         <v>360</v>
       </c>
-      <c r="S123" s="19">
+      <c r="S123" s="16">
         <v>1.0</v>
       </c>
-      <c r="T123" s="20" t="s">
+      <c r="T123" s="17" t="s">
         <v>554</v>
       </c>
-      <c r="U123" s="21"/>
-      <c r="V123" s="21"/>
-      <c r="W123" s="21"/>
-      <c r="X123" s="21"/>
-      <c r="Y123" s="21"/>
-      <c r="Z123" s="21"/>
-      <c r="AA123" s="21"/>
-      <c r="AB123" s="21"/>
-    </row>
-    <row r="124" ht="15.75" hidden="1" customHeight="1">
+      <c r="U123" s="18"/>
+      <c r="V123" s="18"/>
+      <c r="W123" s="18"/>
+      <c r="X123" s="18"/>
+      <c r="Y123" s="18"/>
+      <c r="Z123" s="18"/>
+      <c r="AA123" s="18"/>
+      <c r="AB123" s="18"/>
+    </row>
+    <row r="124" ht="15.75" customHeight="1">
       <c r="A124" s="8">
         <v>3.856280479E9</v>
       </c>
@@ -9457,7 +9519,7 @@
       <c r="AA125" s="18"/>
       <c r="AB125" s="18"/>
     </row>
-    <row r="126" ht="15.75" hidden="1" customHeight="1">
+    <row r="126" ht="15.75" customHeight="1">
       <c r="A126" s="8">
         <v>2.609260641E9</v>
       </c>
@@ -9576,7 +9638,7 @@
       <c r="AA127" s="18"/>
       <c r="AB127" s="18"/>
     </row>
-    <row r="128" ht="15.75" hidden="1" customHeight="1">
+    <row r="128" ht="15.75" customHeight="1">
       <c r="A128" s="8">
         <v>6.66050348E8</v>
       </c>
@@ -9662,13 +9724,13 @@
       <c r="L129" s="16">
         <v>38.0</v>
       </c>
-      <c r="M129" s="22" t="s">
+      <c r="M129" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="N129" s="22" t="s">
+      <c r="N129" s="19" t="s">
         <v>578</v>
       </c>
-      <c r="O129" s="22" t="s">
+      <c r="O129" s="19" t="s">
         <v>579</v>
       </c>
       <c r="P129" s="17" t="s">
@@ -9695,7 +9757,7 @@
       <c r="AA129" s="18"/>
       <c r="AB129" s="18"/>
     </row>
-    <row r="130" ht="15.75" hidden="1" customHeight="1">
+    <row r="130" ht="15.75" customHeight="1">
       <c r="A130" s="8">
         <v>1.637690235E9</v>
       </c>
@@ -9814,7 +9876,7 @@
       <c r="AA131" s="18"/>
       <c r="AB131" s="18"/>
     </row>
-    <row r="132" ht="15.75" hidden="1" customHeight="1">
+    <row r="132" ht="15.75" customHeight="1">
       <c r="A132" s="8">
         <v>2.155422499E9</v>
       </c>
@@ -9933,7 +9995,7 @@
       <c r="AA133" s="18"/>
       <c r="AB133" s="18"/>
     </row>
-    <row r="134" ht="15.75" hidden="1" customHeight="1">
+    <row r="134" ht="15.75" customHeight="1">
       <c r="A134" s="8">
         <v>3.309250332E9</v>
       </c>
@@ -10052,7 +10114,7 @@
       <c r="AA135" s="18"/>
       <c r="AB135" s="18"/>
     </row>
-    <row r="136" ht="15.75" hidden="1" customHeight="1">
+    <row r="136" ht="15.75" customHeight="1">
       <c r="A136" s="8">
         <v>3.625722965E9</v>
       </c>
@@ -10171,7 +10233,7 @@
       <c r="AA137" s="16"/>
       <c r="AB137" s="16"/>
     </row>
-    <row r="138" ht="15.75" hidden="1" customHeight="1">
+    <row r="138" ht="15.75" customHeight="1">
       <c r="A138" s="8">
         <v>4.278392816E9</v>
       </c>
@@ -10290,7 +10352,7 @@
       <c r="AA139" s="18"/>
       <c r="AB139" s="18"/>
     </row>
-    <row r="140" ht="15.75" hidden="1" customHeight="1">
+    <row r="140" ht="15.75" customHeight="1">
       <c r="A140" s="8">
         <v>5.66043228E8</v>
       </c>
@@ -10409,7 +10471,7 @@
       <c r="AA141" s="18"/>
       <c r="AB141" s="18"/>
     </row>
-    <row r="142" ht="15.75" hidden="1" customHeight="1">
+    <row r="142" ht="15.75" customHeight="1">
       <c r="A142" s="8">
         <v>8.53680639E8</v>
       </c>
@@ -10528,7 +10590,7 @@
       <c r="AA143" s="18"/>
       <c r="AB143" s="18"/>
     </row>
-    <row r="144" ht="15.75" hidden="1" customHeight="1">
+    <row r="144" ht="15.75" customHeight="1">
       <c r="A144" s="8">
         <v>3.637456466E9</v>
       </c>
@@ -10647,7 +10709,7 @@
       <c r="AA145" s="18"/>
       <c r="AB145" s="18"/>
     </row>
-    <row r="146" ht="15.75" hidden="1" customHeight="1">
+    <row r="146" ht="15.75" customHeight="1">
       <c r="A146" s="8">
         <v>3.754172825E9</v>
       </c>
@@ -10697,76 +10759,76 @@
       </c>
     </row>
     <row r="147" ht="15.75" customHeight="1">
-      <c r="A147" s="16">
+      <c r="A147" s="20">
         <v>1.296637108E9</v>
       </c>
-      <c r="B147" s="16" t="s">
+      <c r="B147" s="20" t="s">
         <v>656</v>
       </c>
-      <c r="C147" s="16" t="s">
+      <c r="C147" s="20" t="s">
         <v>657</v>
       </c>
-      <c r="D147" s="16">
+      <c r="D147" s="20">
         <v>2019.0</v>
       </c>
-      <c r="E147" s="16" t="s">
+      <c r="E147" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="F147" s="16" t="s">
+      <c r="F147" s="20" t="s">
         <v>658</v>
       </c>
-      <c r="G147" s="16" t="s">
+      <c r="G147" s="20" t="s">
         <v>659</v>
       </c>
-      <c r="H147" s="16" t="s">
+      <c r="H147" s="20" t="s">
         <v>192</v>
       </c>
-      <c r="I147" s="16" t="s">
+      <c r="I147" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="J147" s="16" t="s">
+      <c r="J147" s="20" t="s">
         <v>272</v>
       </c>
-      <c r="K147" s="16" t="s">
+      <c r="K147" s="20" t="s">
         <v>273</v>
       </c>
-      <c r="L147" s="16">
+      <c r="L147" s="20">
         <v>47.0</v>
       </c>
-      <c r="M147" s="17" t="s">
+      <c r="M147" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="N147" s="17" t="s">
+      <c r="N147" s="21" t="s">
         <v>660</v>
       </c>
-      <c r="O147" s="17" t="s">
+      <c r="O147" s="21" t="s">
         <v>661</v>
       </c>
-      <c r="P147" s="17" t="s">
+      <c r="P147" s="21" t="s">
         <v>662</v>
       </c>
-      <c r="Q147" s="17" t="s">
+      <c r="Q147" s="21" t="s">
         <v>663</v>
       </c>
-      <c r="R147" s="16" t="s">
+      <c r="R147" s="20" t="s">
         <v>360</v>
       </c>
-      <c r="S147" s="16">
+      <c r="S147" s="20">
         <v>1.0</v>
       </c>
-      <c r="T147" s="17" t="s">
+      <c r="T147" s="21" t="s">
         <v>664</v>
       </c>
-      <c r="U147" s="18"/>
-      <c r="V147" s="18"/>
-      <c r="W147" s="18"/>
-      <c r="X147" s="18"/>
-      <c r="Y147" s="18"/>
-      <c r="Z147" s="18"/>
-      <c r="AA147" s="18"/>
-      <c r="AB147" s="18"/>
-    </row>
-    <row r="148" ht="15.75" hidden="1" customHeight="1">
+      <c r="U147" s="22"/>
+      <c r="V147" s="22"/>
+      <c r="W147" s="22"/>
+      <c r="X147" s="22"/>
+      <c r="Y147" s="22"/>
+      <c r="Z147" s="22"/>
+      <c r="AA147" s="22"/>
+      <c r="AB147" s="22"/>
+    </row>
+    <row r="148" ht="15.75" customHeight="1">
       <c r="A148" s="8">
         <v>1.296637108E9</v>
       </c>
@@ -29582,18 +29644,7 @@
       <c r="T1001" s="23"/>
     </row>
   </sheetData>
-  <autoFilter ref="$A$1:$AB$148">
-    <filterColumn colId="18">
-      <filters blank="1">
-        <filter val="1"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="17">
-      <filters blank="1">
-        <filter val="Clayton"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="$A$1:$AB$148"/>
   <printOptions/>
   <pageMargins bottom="1.0" footer="0.0" header="0.0" left="0.75" right="0.75" top="1.0"/>
   <pageSetup orientation="landscape"/>
@@ -29750,7 +29801,7 @@
       <c r="AC2" s="7"/>
       <c r="AD2" s="7"/>
     </row>
-    <row r="3" hidden="1">
+    <row r="3">
       <c r="A3" s="8">
         <v>1.326191931E9</v>
       </c>
@@ -29801,7 +29852,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="4" hidden="1">
+    <row r="4">
       <c r="A4" s="8">
         <v>1.326191931E9</v>
       </c>
@@ -29852,7 +29903,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="5" hidden="1">
+    <row r="5">
       <c r="A5" s="8">
         <v>1.469065963E9</v>
       </c>
@@ -29903,7 +29954,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="6" hidden="1">
+    <row r="6">
       <c r="A6" s="8">
         <v>1.469065963E9</v>
       </c>
@@ -29954,7 +30005,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="7" hidden="1">
+    <row r="7">
       <c r="A7" s="8">
         <v>1.598166515E9</v>
       </c>
@@ -30005,7 +30056,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="8" hidden="1">
+    <row r="8">
       <c r="A8" s="8">
         <v>1.598166515E9</v>
       </c>
@@ -30056,7 +30107,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="9" hidden="1">
+    <row r="9">
       <c r="A9" s="8">
         <v>1.877483551E9</v>
       </c>
@@ -30107,7 +30158,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="10" hidden="1">
+    <row r="10">
       <c r="A10" s="8">
         <v>1.877483551E9</v>
       </c>
@@ -30158,7 +30209,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="11" hidden="1">
+    <row r="11">
       <c r="A11" s="8">
         <v>2.000036002E9</v>
       </c>
@@ -30209,7 +30260,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="12" hidden="1">
+    <row r="12">
       <c r="A12" s="8">
         <v>2.000036002E9</v>
       </c>
@@ -30260,7 +30311,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="13" hidden="1">
+    <row r="13">
       <c r="A13" s="8">
         <v>2.070224207E9</v>
       </c>
@@ -30311,7 +30362,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="14" hidden="1">
+    <row r="14">
       <c r="A14" s="8">
         <v>2.070224207E9</v>
       </c>
@@ -30362,7 +30413,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="15" hidden="1">
+    <row r="15">
       <c r="A15" s="8">
         <v>2.634033325E9</v>
       </c>
@@ -30413,7 +30464,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="16" hidden="1">
+    <row r="16">
       <c r="A16" s="8">
         <v>2.634033325E9</v>
       </c>
@@ -30464,7 +30515,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="17" hidden="1">
+    <row r="17">
       <c r="A17" s="8">
         <v>3.051560548E9</v>
       </c>
@@ -30515,7 +30566,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="18" hidden="1">
+    <row r="18">
       <c r="A18" s="8">
         <v>3.051560548E9</v>
       </c>
@@ -30566,7 +30617,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="19" hidden="1">
+    <row r="19">
       <c r="A19" s="8">
         <v>3.339002981E9</v>
       </c>
@@ -30617,7 +30668,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="20" hidden="1">
+    <row r="20">
       <c r="A20" s="8">
         <v>3.339002981E9</v>
       </c>
@@ -30668,7 +30719,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="21" hidden="1">
+    <row r="21">
       <c r="A21" s="8">
         <v>3.408664396E9</v>
       </c>
@@ -30719,7 +30770,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="22" ht="15.75" hidden="1" customHeight="1">
+    <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="8">
         <v>3.408664396E9</v>
       </c>
@@ -30770,7 +30821,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="23" ht="15.75" hidden="1" customHeight="1">
+    <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="8">
         <v>8.04659204E8</v>
       </c>
@@ -30821,7 +30872,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="24" ht="15.75" hidden="1" customHeight="1">
+    <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="8">
         <v>8.04659204E8</v>
       </c>
@@ -30872,7 +30923,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="25" ht="15.75" hidden="1" customHeight="1">
+    <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="8">
         <v>1.581261659E9</v>
       </c>
@@ -30923,7 +30974,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="26" ht="15.75" hidden="1" customHeight="1">
+    <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="8">
         <v>1.581261659E9</v>
       </c>
@@ -30974,7 +31025,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="27" ht="15.75" hidden="1" customHeight="1">
+    <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="8">
         <v>2.836996318E9</v>
       </c>
@@ -31025,7 +31076,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="28" ht="15.75" hidden="1" customHeight="1">
+    <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="8">
         <v>2.836996318E9</v>
       </c>
@@ -31076,7 +31127,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="29" ht="15.75" hidden="1" customHeight="1">
+    <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="8">
         <v>3.2184286E7</v>
       </c>
@@ -31127,7 +31178,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="30" ht="15.75" hidden="1" customHeight="1">
+    <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="8">
         <v>3.2184286E7</v>
       </c>
@@ -31178,7 +31229,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="31" ht="15.75" hidden="1" customHeight="1">
+    <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="8">
         <v>4.33919853E8</v>
       </c>
@@ -31229,7 +31280,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="32" ht="15.75" hidden="1" customHeight="1">
+    <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="8">
         <v>4.33919853E8</v>
       </c>
@@ -31280,7 +31331,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="33" ht="15.75" hidden="1" customHeight="1">
+    <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="8">
         <v>4.83140962E8</v>
       </c>
@@ -31331,7 +31382,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="34" ht="15.75" hidden="1" customHeight="1">
+    <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="8">
         <v>4.83140962E8</v>
       </c>
@@ -31382,7 +31433,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="35" ht="15.75" hidden="1" customHeight="1">
+    <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="8">
         <v>3.308658121E9</v>
       </c>
@@ -31433,7 +31484,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="36" ht="15.75" hidden="1" customHeight="1">
+    <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="8">
         <v>3.308658121E9</v>
       </c>
@@ -31484,7 +31535,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="37" ht="15.75" hidden="1" customHeight="1">
+    <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="8">
         <v>1.847468084E9</v>
       </c>
@@ -31535,7 +31586,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="38" ht="15.75" hidden="1" customHeight="1">
+    <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="8">
         <v>1.847468084E9</v>
       </c>
@@ -31586,7 +31637,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="39" ht="15.75" hidden="1" customHeight="1">
+    <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="8">
         <v>2.345021698E9</v>
       </c>
@@ -31637,7 +31688,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="40" ht="15.75" hidden="1" customHeight="1">
+    <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="8">
         <v>2.345021698E9</v>
       </c>
@@ -31688,7 +31739,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="41" ht="15.75" hidden="1" customHeight="1">
+    <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="8">
         <v>3.796643912E9</v>
       </c>
@@ -31742,7 +31793,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="42" ht="15.75" hidden="1" customHeight="1">
+    <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="8">
         <v>3.796643912E9</v>
       </c>
@@ -31793,7 +31844,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="43" ht="15.75" hidden="1" customHeight="1">
+    <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="8">
         <v>2.05660768E8</v>
       </c>
@@ -31844,7 +31895,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="44" ht="15.75" hidden="1" customHeight="1">
+    <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="8">
         <v>2.05660768E8</v>
       </c>
@@ -31895,7 +31946,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="45" ht="15.75" hidden="1" customHeight="1">
+    <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="8">
         <v>2.18163761E9</v>
       </c>
@@ -31946,7 +31997,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="46" ht="15.75" hidden="1" customHeight="1">
+    <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="8">
         <v>2.18163761E9</v>
       </c>
@@ -31997,7 +32048,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="47" ht="15.75" hidden="1" customHeight="1">
+    <row r="47" ht="15.75" customHeight="1">
       <c r="A47" s="8">
         <v>4.035649049E9</v>
       </c>
@@ -32048,7 +32099,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="48" ht="15.75" hidden="1" customHeight="1">
+    <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="8">
         <v>4.035649049E9</v>
       </c>
@@ -32099,7 +32150,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="49" ht="15.75" hidden="1" customHeight="1">
+    <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="8">
         <v>1.019093033E9</v>
       </c>
@@ -32150,7 +32201,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="50" ht="15.75" hidden="1" customHeight="1">
+    <row r="50" ht="15.75" customHeight="1">
       <c r="A50" s="8">
         <v>1.019093033E9</v>
       </c>
@@ -32201,7 +32252,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="51" ht="15.75" hidden="1" customHeight="1">
+    <row r="51" ht="15.75" customHeight="1">
       <c r="A51" s="8">
         <v>2.936220551E9</v>
       </c>
@@ -32252,7 +32303,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="52" ht="15.75" hidden="1" customHeight="1">
+    <row r="52" ht="15.75" customHeight="1">
       <c r="A52" s="8">
         <v>2.936220551E9</v>
       </c>
@@ -32303,7 +32354,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="53" ht="15.75" hidden="1" customHeight="1">
+    <row r="53" ht="15.75" customHeight="1">
       <c r="A53" s="8">
         <v>1.886134458E9</v>
       </c>
@@ -32354,7 +32405,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="54" ht="15.75" hidden="1" customHeight="1">
+    <row r="54" ht="15.75" customHeight="1">
       <c r="A54" s="8">
         <v>1.886134458E9</v>
       </c>
@@ -32405,7 +32456,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="55" ht="15.75" hidden="1" customHeight="1">
+    <row r="55" ht="15.75" customHeight="1">
       <c r="A55" s="8">
         <v>2.879332689E9</v>
       </c>
@@ -32456,7 +32507,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="56" ht="15.75" hidden="1" customHeight="1">
+    <row r="56" ht="15.75" customHeight="1">
       <c r="A56" s="8">
         <v>2.879332689E9</v>
       </c>
@@ -32507,7 +32558,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="57" ht="15.75" hidden="1" customHeight="1">
+    <row r="57" ht="15.75" customHeight="1">
       <c r="A57" s="8">
         <v>3.146393211E9</v>
       </c>
@@ -32558,7 +32609,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="58" ht="15.75" hidden="1" customHeight="1">
+    <row r="58" ht="15.75" customHeight="1">
       <c r="A58" s="8">
         <v>3.146393211E9</v>
       </c>
@@ -32609,7 +32660,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="59" ht="15.75" hidden="1" customHeight="1">
+    <row r="59" ht="15.75" customHeight="1">
       <c r="A59" s="8">
         <v>3.809293172E9</v>
       </c>
@@ -32660,7 +32711,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="60" ht="15.75" hidden="1" customHeight="1">
+    <row r="60" ht="15.75" customHeight="1">
       <c r="A60" s="8">
         <v>3.809293172E9</v>
       </c>
@@ -32711,7 +32762,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="61" ht="15.75" hidden="1" customHeight="1">
+    <row r="61" ht="15.75" customHeight="1">
       <c r="A61" s="8">
         <v>4.019205162E9</v>
       </c>
@@ -32762,7 +32813,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="62" ht="15.75" hidden="1" customHeight="1">
+    <row r="62" ht="15.75" customHeight="1">
       <c r="A62" s="8">
         <v>4.019205162E9</v>
       </c>
@@ -32813,7 +32864,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="63" ht="15.75" hidden="1" customHeight="1">
+    <row r="63" ht="15.75" customHeight="1">
       <c r="A63" s="8">
         <v>4.27781205E9</v>
       </c>
@@ -32864,7 +32915,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="64" ht="15.75" hidden="1" customHeight="1">
+    <row r="64" ht="15.75" customHeight="1">
       <c r="A64" s="8">
         <v>4.27781205E9</v>
       </c>
@@ -32915,7 +32966,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="65" ht="15.75" hidden="1" customHeight="1">
+    <row r="65" ht="15.75" customHeight="1">
       <c r="A65" s="8">
         <v>1.609706685E9</v>
       </c>
@@ -32966,7 +33017,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="66" ht="15.75" hidden="1" customHeight="1">
+    <row r="66" ht="15.75" customHeight="1">
       <c r="A66" s="8">
         <v>1.609706685E9</v>
       </c>
@@ -33017,7 +33068,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="67" ht="15.75" hidden="1" customHeight="1">
+    <row r="67" ht="15.75" customHeight="1">
       <c r="A67" s="8">
         <v>3.398902089E9</v>
       </c>
@@ -33068,7 +33119,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="68" ht="15.75" hidden="1" customHeight="1">
+    <row r="68" ht="15.75" customHeight="1">
       <c r="A68" s="8">
         <v>3.398902089E9</v>
       </c>
@@ -33119,7 +33170,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="69" ht="15.75" hidden="1" customHeight="1">
+    <row r="69" ht="15.75" customHeight="1">
       <c r="A69" s="8">
         <v>3.093310941E9</v>
       </c>
@@ -33170,7 +33221,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="70" ht="15.75" hidden="1" customHeight="1">
+    <row r="70" ht="15.75" customHeight="1">
       <c r="A70" s="8">
         <v>3.093310941E9</v>
       </c>
@@ -33221,7 +33272,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="71" ht="15.75" hidden="1" customHeight="1">
+    <row r="71" ht="15.75" customHeight="1">
       <c r="A71" s="8">
         <v>1.576545447E9</v>
       </c>
@@ -33272,7 +33323,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="72" ht="15.75" hidden="1" customHeight="1">
+    <row r="72" ht="15.75" customHeight="1">
       <c r="A72" s="8">
         <v>1.576545447E9</v>
       </c>
@@ -33323,7 +33374,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="73" ht="15.75" hidden="1" customHeight="1">
+    <row r="73" ht="15.75" customHeight="1">
       <c r="A73" s="8">
         <v>3.796180663E9</v>
       </c>
@@ -33374,7 +33425,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="74" ht="15.75" hidden="1" customHeight="1">
+    <row r="74" ht="15.75" customHeight="1">
       <c r="A74" s="8">
         <v>3.796180663E9</v>
       </c>
@@ -33425,7 +33476,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="75" ht="15.75" hidden="1" customHeight="1">
+    <row r="75" ht="15.75" customHeight="1">
       <c r="A75" s="8">
         <v>1.770989706E9</v>
       </c>
@@ -33476,7 +33527,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="76" ht="15.75" hidden="1" customHeight="1">
+    <row r="76" ht="15.75" customHeight="1">
       <c r="A76" s="8">
         <v>1.770989706E9</v>
       </c>
@@ -33527,7 +33578,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="77" ht="15.75" hidden="1" customHeight="1">
+    <row r="77" ht="15.75" customHeight="1">
       <c r="A77" s="8">
         <v>2.456887548E9</v>
       </c>
@@ -33578,7 +33629,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="78" ht="15.75" hidden="1" customHeight="1">
+    <row r="78" ht="15.75" customHeight="1">
       <c r="A78" s="8">
         <v>2.456887548E9</v>
       </c>
@@ -33629,7 +33680,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="79" ht="15.75" hidden="1" customHeight="1">
+    <row r="79" ht="15.75" customHeight="1">
       <c r="A79" s="8">
         <v>5.18268671E8</v>
       </c>
@@ -33680,7 +33731,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="80" ht="15.75" hidden="1" customHeight="1">
+    <row r="80" ht="15.75" customHeight="1">
       <c r="A80" s="8">
         <v>5.18268671E8</v>
       </c>
@@ -33731,7 +33782,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="81" ht="15.75" hidden="1" customHeight="1">
+    <row r="81" ht="15.75" customHeight="1">
       <c r="A81" s="8">
         <v>9.57160695E8</v>
       </c>
@@ -33782,7 +33833,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="82" ht="15.75" hidden="1" customHeight="1">
+    <row r="82" ht="15.75" customHeight="1">
       <c r="A82" s="8">
         <v>9.57160695E8</v>
       </c>
@@ -33833,7 +33884,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="83" ht="15.75" hidden="1" customHeight="1">
+    <row r="83" ht="15.75" customHeight="1">
       <c r="A83" s="8">
         <v>3.00954867E9</v>
       </c>
@@ -33884,7 +33935,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="84" ht="15.75" hidden="1" customHeight="1">
+    <row r="84" ht="15.75" customHeight="1">
       <c r="A84" s="8">
         <v>3.00954867E9</v>
       </c>
@@ -33935,7 +33986,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="85" ht="15.75" hidden="1" customHeight="1">
+    <row r="85" ht="15.75" customHeight="1">
       <c r="A85" s="8">
         <v>3.448122334E9</v>
       </c>
@@ -33986,7 +34037,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="86" ht="15.75" hidden="1" customHeight="1">
+    <row r="86" ht="15.75" customHeight="1">
       <c r="A86" s="8">
         <v>3.448122334E9</v>
       </c>
@@ -34037,7 +34088,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="87" ht="15.75" hidden="1" customHeight="1">
+    <row r="87" ht="15.75" customHeight="1">
       <c r="A87" s="8">
         <v>2.497456347E9</v>
       </c>
@@ -34088,7 +34139,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="88" ht="15.75" hidden="1" customHeight="1">
+    <row r="88" ht="15.75" customHeight="1">
       <c r="A88" s="8">
         <v>2.497456347E9</v>
       </c>
@@ -34139,7 +34190,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="89" ht="15.75" hidden="1" customHeight="1">
+    <row r="89" ht="15.75" customHeight="1">
       <c r="A89" s="8">
         <v>3.660066725E9</v>
       </c>
@@ -34190,7 +34241,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="90" ht="15.75" hidden="1" customHeight="1">
+    <row r="90" ht="15.75" customHeight="1">
       <c r="A90" s="8">
         <v>3.660066725E9</v>
       </c>
@@ -34241,7 +34292,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="91" ht="15.75" hidden="1" customHeight="1">
+    <row r="91" ht="15.75" customHeight="1">
       <c r="A91" s="8">
         <v>3.783339081E9</v>
       </c>
@@ -34292,7 +34343,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="92" ht="15.75" hidden="1" customHeight="1">
+    <row r="92" ht="15.75" customHeight="1">
       <c r="A92" s="8">
         <v>3.783339081E9</v>
       </c>
@@ -34343,7 +34394,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="93" ht="15.75" hidden="1" customHeight="1">
+    <row r="93" ht="15.75" customHeight="1">
       <c r="A93" s="8">
         <v>3.095923626E9</v>
       </c>
@@ -34394,7 +34445,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="94" ht="15.75" hidden="1" customHeight="1">
+    <row r="94" ht="15.75" customHeight="1">
       <c r="A94" s="8">
         <v>3.095923626E9</v>
       </c>
@@ -34445,7 +34496,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="95" ht="15.75" hidden="1" customHeight="1">
+    <row r="95" ht="15.75" customHeight="1">
       <c r="A95" s="8">
         <v>8.5990093E7</v>
       </c>
@@ -34496,7 +34547,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="96" ht="15.75" hidden="1" customHeight="1">
+    <row r="96" ht="15.75" customHeight="1">
       <c r="A96" s="8">
         <v>8.5990093E7</v>
       </c>
@@ -34547,7 +34598,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="97" ht="15.75" hidden="1" customHeight="1">
+    <row r="97" ht="15.75" customHeight="1">
       <c r="A97" s="8">
         <v>8.6191824E7</v>
       </c>
@@ -34598,7 +34649,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="98" ht="15.75" hidden="1" customHeight="1">
+    <row r="98" ht="15.75" customHeight="1">
       <c r="A98" s="8">
         <v>8.6191824E7</v>
       </c>
@@ -34649,7 +34700,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="99" ht="15.75" hidden="1" customHeight="1">
+    <row r="99" ht="15.75" customHeight="1">
       <c r="A99" s="8">
         <v>8.18492192E8</v>
       </c>
@@ -34700,7 +34751,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="100" ht="15.75" hidden="1" customHeight="1">
+    <row r="100" ht="15.75" customHeight="1">
       <c r="A100" s="8">
         <v>8.18492192E8</v>
       </c>
@@ -34751,7 +34802,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="101" ht="15.75" hidden="1" customHeight="1">
+    <row r="101" ht="15.75" customHeight="1">
       <c r="A101" s="8">
         <v>1.47203129E8</v>
       </c>
@@ -34802,7 +34853,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="102" ht="15.75" hidden="1" customHeight="1">
+    <row r="102" ht="15.75" customHeight="1">
       <c r="A102" s="8">
         <v>1.47203129E8</v>
       </c>
@@ -34853,7 +34904,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="103" ht="15.75" hidden="1" customHeight="1">
+    <row r="103" ht="15.75" customHeight="1">
       <c r="A103" s="8">
         <v>1.23412197E8</v>
       </c>
@@ -34904,7 +34955,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="104" ht="15.75" hidden="1" customHeight="1">
+    <row r="104" ht="15.75" customHeight="1">
       <c r="A104" s="8">
         <v>1.23412197E8</v>
       </c>
@@ -34955,7 +35006,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="105" ht="15.75" hidden="1" customHeight="1">
+    <row r="105" ht="15.75" customHeight="1">
       <c r="A105" s="8">
         <v>1.118315889E9</v>
       </c>
@@ -35006,7 +35057,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="106" ht="15.75" hidden="1" customHeight="1">
+    <row r="106" ht="15.75" customHeight="1">
       <c r="A106" s="8">
         <v>1.118315889E9</v>
       </c>
@@ -35057,7 +35108,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="107" ht="15.75" hidden="1" customHeight="1">
+    <row r="107" ht="15.75" customHeight="1">
       <c r="A107" s="8">
         <v>1.315379489E9</v>
       </c>
@@ -35108,7 +35159,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="108" ht="15.75" hidden="1" customHeight="1">
+    <row r="108" ht="15.75" customHeight="1">
       <c r="A108" s="8">
         <v>1.315379489E9</v>
       </c>
@@ -35159,7 +35210,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="109" ht="15.75" hidden="1" customHeight="1">
+    <row r="109" ht="15.75" customHeight="1">
       <c r="A109" s="8">
         <v>1.374035721E9</v>
       </c>
@@ -35210,7 +35261,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="110" ht="15.75" hidden="1" customHeight="1">
+    <row r="110" ht="15.75" customHeight="1">
       <c r="A110" s="8">
         <v>1.374035721E9</v>
       </c>
@@ -35261,7 +35312,7 @@
         <v>2.0</v>
       </c>
     </row>
-    <row r="111" ht="15.75" hidden="1" customHeight="1">
+    <row r="111" ht="15.75" customHeight="1">
       <c r="A111" s="8">
         <v>1.426267857E9</v>
       </c>
@@ -35312,7 +35363,7 @@
         <v>1.0</v>
       </c>
     </row>
-    <row r="112" ht="30.0" hidden="1" customHeight="1">
+    <row r="112" ht="30.0" customHeight="1">
       <c r="A112" s="8">
         <v>1.426267857E9</v>
       </c>
@@ -35439,7 +35490,7 @@
       <c r="AC113" s="26"/>
       <c r="AD113" s="26"/>
     </row>
-    <row r="114" ht="15.75" hidden="1" customHeight="1">
+    <row r="114" ht="15.75" customHeight="1">
       <c r="A114" s="8">
         <v>2.055153191E9</v>
       </c>
@@ -35566,7 +35617,7 @@
       <c r="AC115" s="26"/>
       <c r="AD115" s="26"/>
     </row>
-    <row r="116" ht="15.75" hidden="1" customHeight="1">
+    <row r="116" ht="15.75" customHeight="1">
       <c r="A116" s="8">
         <v>2.273914836E9</v>
       </c>
@@ -35693,7 +35744,7 @@
       <c r="AC117" s="26"/>
       <c r="AD117" s="26"/>
     </row>
-    <row r="118" ht="15.75" hidden="1" customHeight="1">
+    <row r="118" ht="15.75" customHeight="1">
       <c r="A118" s="8">
         <v>1.763513559E9</v>
       </c>
@@ -35820,7 +35871,7 @@
       <c r="AC119" s="26"/>
       <c r="AD119" s="26"/>
     </row>
-    <row r="120" ht="15.75" hidden="1" customHeight="1">
+    <row r="120" ht="15.75" customHeight="1">
       <c r="A120" s="8">
         <v>1.345598079E9</v>
       </c>
@@ -35947,7 +35998,7 @@
       <c r="AC121" s="26"/>
       <c r="AD121" s="26"/>
     </row>
-    <row r="122" ht="15.75" hidden="1" customHeight="1">
+    <row r="122" ht="15.75" customHeight="1">
       <c r="A122" s="8">
         <v>3.135645357E9</v>
       </c>
@@ -35999,68 +36050,82 @@
       </c>
     </row>
     <row r="123" ht="15.75" customHeight="1">
-      <c r="A123" s="19">
+      <c r="A123" s="24">
         <v>3.856280479E9</v>
       </c>
-      <c r="B123" s="19" t="s">
+      <c r="B123" s="24" t="s">
         <v>548</v>
       </c>
-      <c r="C123" s="19" t="s">
+      <c r="C123" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="D123" s="19">
+      <c r="D123" s="24">
         <v>2021.0</v>
       </c>
-      <c r="E123" s="19" t="s">
+      <c r="E123" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="F123" s="19" t="s">
+      <c r="F123" s="24" t="s">
         <v>412</v>
       </c>
-      <c r="G123" s="19" t="s">
+      <c r="G123" s="24" t="s">
         <v>549</v>
       </c>
-      <c r="H123" s="19" t="s">
+      <c r="H123" s="24" t="s">
         <v>550</v>
       </c>
-      <c r="I123" s="19" t="s">
+      <c r="I123" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="J123" s="19" t="s">
+      <c r="J123" s="24" t="s">
         <v>290</v>
       </c>
-      <c r="K123" s="19" t="s">
+      <c r="K123" s="24" t="s">
         <v>291</v>
       </c>
-      <c r="L123" s="19">
+      <c r="L123" s="24">
         <v>35.0</v>
       </c>
-      <c r="M123" s="20"/>
-      <c r="N123" s="20"/>
-      <c r="O123" s="20"/>
-      <c r="P123" s="20"/>
-      <c r="Q123" s="20"/>
-      <c r="R123" s="20"/>
-      <c r="S123" s="20"/>
-      <c r="T123" s="19" t="s">
+      <c r="M123" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="N123" s="25" t="s">
+        <v>683</v>
+      </c>
+      <c r="O123" s="25" t="s">
+        <v>686</v>
+      </c>
+      <c r="P123" s="25" t="s">
+        <v>679</v>
+      </c>
+      <c r="Q123" s="25" t="s">
+        <v>680</v>
+      </c>
+      <c r="R123" s="25" t="s">
+        <v>675</v>
+      </c>
+      <c r="S123" s="25" t="s">
+        <v>553</v>
+      </c>
+      <c r="T123" s="24" t="s">
         <v>360</v>
       </c>
-      <c r="U123" s="19">
+      <c r="U123" s="24">
         <v>1.0</v>
       </c>
-      <c r="V123" s="20" t="s">
-        <v>554</v>
-      </c>
-      <c r="W123" s="21"/>
-      <c r="X123" s="21"/>
-      <c r="Y123" s="21"/>
-      <c r="Z123" s="21"/>
-      <c r="AA123" s="21"/>
-      <c r="AB123" s="21"/>
-      <c r="AC123" s="21"/>
-      <c r="AD123" s="21"/>
-    </row>
-    <row r="124" ht="15.75" hidden="1" customHeight="1">
+      <c r="V123" s="25" t="s">
+        <v>695</v>
+      </c>
+      <c r="W123" s="26"/>
+      <c r="X123" s="26"/>
+      <c r="Y123" s="26"/>
+      <c r="Z123" s="26"/>
+      <c r="AA123" s="26"/>
+      <c r="AB123" s="26"/>
+      <c r="AC123" s="26"/>
+      <c r="AD123" s="26"/>
+    </row>
+    <row r="124" ht="15.75" customHeight="1">
       <c r="A124" s="8">
         <v>3.856280479E9</v>
       </c>
@@ -36112,60 +36177,82 @@
       </c>
     </row>
     <row r="125" ht="15.75" customHeight="1">
-      <c r="A125" s="23">
+      <c r="A125" s="24">
         <v>2.609260641E9</v>
       </c>
-      <c r="B125" s="23" t="s">
+      <c r="B125" s="24" t="s">
         <v>555</v>
       </c>
-      <c r="C125" s="23" t="s">
+      <c r="C125" s="24" t="s">
         <v>199</v>
       </c>
-      <c r="D125" s="23">
+      <c r="D125" s="24">
         <v>2022.0</v>
       </c>
-      <c r="E125" s="23" t="s">
+      <c r="E125" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="F125" s="23" t="s">
+      <c r="F125" s="24" t="s">
         <v>556</v>
       </c>
-      <c r="G125" s="23" t="s">
+      <c r="G125" s="24" t="s">
         <v>557</v>
       </c>
-      <c r="H125" s="23" t="s">
+      <c r="H125" s="24" t="s">
         <v>192</v>
       </c>
-      <c r="I125" s="23" t="s">
+      <c r="I125" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="J125" s="23" t="s">
+      <c r="J125" s="24" t="s">
         <v>558</v>
       </c>
-      <c r="K125" s="23" t="s">
+      <c r="K125" s="24" t="s">
         <v>559</v>
       </c>
-      <c r="L125" s="23">
+      <c r="L125" s="24">
         <v>36.0</v>
       </c>
-      <c r="M125" s="10"/>
-      <c r="N125" s="10"/>
-      <c r="O125" s="10"/>
-      <c r="P125" s="10"/>
-      <c r="Q125" s="10"/>
-      <c r="R125" s="10"/>
-      <c r="S125" s="10"/>
-      <c r="T125" s="23" t="s">
+      <c r="M125" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="N125" s="25" t="s">
+        <v>560</v>
+      </c>
+      <c r="O125" s="25" t="s">
+        <v>678</v>
+      </c>
+      <c r="P125" s="25" t="s">
+        <v>696</v>
+      </c>
+      <c r="Q125" s="25" t="s">
+        <v>697</v>
+      </c>
+      <c r="R125" s="25" t="s">
+        <v>681</v>
+      </c>
+      <c r="S125" s="25" t="s">
+        <v>698</v>
+      </c>
+      <c r="T125" s="24" t="s">
         <v>360</v>
       </c>
-      <c r="U125" s="23">
+      <c r="U125" s="24">
         <v>1.0</v>
       </c>
-      <c r="V125" s="27" t="s">
+      <c r="V125" s="25" t="s">
         <v>563</v>
       </c>
-    </row>
-    <row r="126" ht="15.75" hidden="1" customHeight="1">
+      <c r="W125" s="26"/>
+      <c r="X125" s="26"/>
+      <c r="Y125" s="26"/>
+      <c r="Z125" s="26"/>
+      <c r="AA125" s="26"/>
+      <c r="AB125" s="26"/>
+      <c r="AC125" s="26"/>
+      <c r="AD125" s="26"/>
+    </row>
+    <row r="126" ht="15.75" customHeight="1">
       <c r="A126" s="8">
         <v>2.609260641E9</v>
       </c>
@@ -36217,60 +36304,82 @@
       </c>
     </row>
     <row r="127" ht="15.75" customHeight="1">
-      <c r="A127" s="23">
+      <c r="A127" s="24">
         <v>6.66050348E8</v>
       </c>
-      <c r="B127" s="23" t="s">
+      <c r="B127" s="24" t="s">
         <v>564</v>
       </c>
-      <c r="C127" s="23" t="s">
+      <c r="C127" s="24" t="s">
         <v>427</v>
       </c>
-      <c r="D127" s="23">
+      <c r="D127" s="24">
         <v>2021.0</v>
       </c>
-      <c r="E127" s="23" t="s">
+      <c r="E127" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="F127" s="23" t="s">
+      <c r="F127" s="24" t="s">
         <v>565</v>
       </c>
-      <c r="G127" s="23" t="s">
+      <c r="G127" s="24" t="s">
         <v>566</v>
       </c>
-      <c r="H127" s="23" t="s">
+      <c r="H127" s="24" t="s">
         <v>192</v>
       </c>
-      <c r="I127" s="23" t="s">
+      <c r="I127" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="J127" s="23" t="s">
+      <c r="J127" s="24" t="s">
         <v>567</v>
       </c>
-      <c r="K127" s="23" t="s">
+      <c r="K127" s="24" t="s">
         <v>568</v>
       </c>
-      <c r="L127" s="23">
+      <c r="L127" s="24">
         <v>37.0</v>
       </c>
-      <c r="M127" s="10"/>
-      <c r="N127" s="10"/>
-      <c r="O127" s="10"/>
-      <c r="P127" s="10"/>
-      <c r="Q127" s="10"/>
-      <c r="R127" s="10"/>
-      <c r="S127" s="10"/>
-      <c r="T127" s="23" t="s">
+      <c r="M127" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="N127" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="O127" s="25" t="s">
+        <v>686</v>
+      </c>
+      <c r="P127" s="25" t="s">
+        <v>696</v>
+      </c>
+      <c r="Q127" s="25" t="s">
+        <v>680</v>
+      </c>
+      <c r="R127" s="25" t="s">
+        <v>681</v>
+      </c>
+      <c r="S127" s="25" t="s">
+        <v>572</v>
+      </c>
+      <c r="T127" s="24" t="s">
         <v>360</v>
       </c>
-      <c r="U127" s="23">
+      <c r="U127" s="24">
         <v>1.0</v>
       </c>
-      <c r="V127" s="27" t="s">
+      <c r="V127" s="25" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="128" ht="15.75" hidden="1" customHeight="1">
+      <c r="W127" s="26"/>
+      <c r="X127" s="26"/>
+      <c r="Y127" s="26"/>
+      <c r="Z127" s="26"/>
+      <c r="AA127" s="26"/>
+      <c r="AB127" s="26"/>
+      <c r="AC127" s="26"/>
+      <c r="AD127" s="26"/>
+    </row>
+    <row r="128" ht="15.75" customHeight="1">
       <c r="A128" s="8">
         <v>6.66050348E8</v>
       </c>
@@ -36322,60 +36431,82 @@
       </c>
     </row>
     <row r="129" ht="15.75" customHeight="1">
-      <c r="A129" s="23">
+      <c r="A129" s="24">
         <v>1.637690235E9</v>
       </c>
-      <c r="B129" s="23" t="s">
+      <c r="B129" s="24" t="s">
         <v>574</v>
       </c>
-      <c r="C129" s="23" t="s">
+      <c r="C129" s="24" t="s">
         <v>112</v>
       </c>
-      <c r="D129" s="23">
+      <c r="D129" s="24">
         <v>2018.0</v>
       </c>
-      <c r="E129" s="23" t="s">
+      <c r="E129" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="F129" s="23" t="s">
+      <c r="F129" s="24" t="s">
         <v>575</v>
       </c>
-      <c r="G129" s="23" t="s">
+      <c r="G129" s="24" t="s">
         <v>576</v>
       </c>
-      <c r="H129" s="23" t="s">
+      <c r="H129" s="24" t="s">
         <v>577</v>
       </c>
-      <c r="I129" s="23" t="s">
+      <c r="I129" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="J129" s="23" t="s">
+      <c r="J129" s="24" t="s">
         <v>346</v>
       </c>
-      <c r="K129" s="23" t="s">
+      <c r="K129" s="24" t="s">
         <v>347</v>
       </c>
-      <c r="L129" s="23">
+      <c r="L129" s="24">
         <v>38.0</v>
       </c>
-      <c r="M129" s="10"/>
-      <c r="N129" s="10"/>
-      <c r="O129" s="10"/>
-      <c r="P129" s="10"/>
-      <c r="Q129" s="10"/>
-      <c r="R129" s="10"/>
-      <c r="S129" s="10"/>
-      <c r="T129" s="23" t="s">
+      <c r="M129" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="N129" s="25" t="s">
+        <v>683</v>
+      </c>
+      <c r="O129" s="25" t="s">
+        <v>678</v>
+      </c>
+      <c r="P129" s="25" t="s">
+        <v>679</v>
+      </c>
+      <c r="Q129" s="25" t="s">
+        <v>699</v>
+      </c>
+      <c r="R129" s="25" t="s">
+        <v>689</v>
+      </c>
+      <c r="S129" s="25" t="s">
+        <v>581</v>
+      </c>
+      <c r="T129" s="24" t="s">
         <v>360</v>
       </c>
-      <c r="U129" s="23">
+      <c r="U129" s="24">
         <v>1.0</v>
       </c>
-      <c r="V129" s="27" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="130" ht="15.75" hidden="1" customHeight="1">
+      <c r="V129" s="25" t="s">
+        <v>700</v>
+      </c>
+      <c r="W129" s="26"/>
+      <c r="X129" s="26"/>
+      <c r="Y129" s="26"/>
+      <c r="Z129" s="26"/>
+      <c r="AA129" s="26"/>
+      <c r="AB129" s="26"/>
+      <c r="AC129" s="26"/>
+      <c r="AD129" s="26"/>
+    </row>
+    <row r="130" ht="15.75" customHeight="1">
       <c r="A130" s="8">
         <v>1.637690235E9</v>
       </c>
@@ -36427,60 +36558,82 @@
       </c>
     </row>
     <row r="131" ht="15.75" customHeight="1">
-      <c r="A131" s="23">
+      <c r="A131" s="24">
         <v>2.155422499E9</v>
       </c>
-      <c r="B131" s="23" t="s">
+      <c r="B131" s="24" t="s">
         <v>583</v>
       </c>
-      <c r="C131" s="23" t="s">
+      <c r="C131" s="24" t="s">
         <v>584</v>
       </c>
-      <c r="D131" s="23">
+      <c r="D131" s="24">
         <v>2022.0</v>
       </c>
-      <c r="E131" s="23" t="s">
+      <c r="E131" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="F131" s="23" t="s">
+      <c r="F131" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="G131" s="23" t="s">
+      <c r="G131" s="24" t="s">
         <v>585</v>
       </c>
-      <c r="H131" s="23" t="s">
+      <c r="H131" s="24" t="s">
         <v>192</v>
       </c>
-      <c r="I131" s="23" t="s">
+      <c r="I131" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="J131" s="23" t="s">
+      <c r="J131" s="24" t="s">
         <v>586</v>
       </c>
-      <c r="K131" s="23" t="s">
+      <c r="K131" s="24" t="s">
         <v>587</v>
       </c>
-      <c r="L131" s="23">
+      <c r="L131" s="24">
         <v>39.0</v>
       </c>
-      <c r="M131" s="10"/>
-      <c r="N131" s="10"/>
-      <c r="O131" s="10"/>
-      <c r="P131" s="10"/>
-      <c r="Q131" s="10"/>
-      <c r="R131" s="10"/>
-      <c r="S131" s="10"/>
-      <c r="T131" s="23" t="s">
+      <c r="M131" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="N131" s="25" t="s">
+        <v>560</v>
+      </c>
+      <c r="O131" s="25" t="s">
+        <v>678</v>
+      </c>
+      <c r="P131" s="25" t="s">
+        <v>687</v>
+      </c>
+      <c r="Q131" s="25" t="s">
+        <v>697</v>
+      </c>
+      <c r="R131" s="25" t="s">
+        <v>681</v>
+      </c>
+      <c r="S131" s="25" t="s">
+        <v>591</v>
+      </c>
+      <c r="T131" s="24" t="s">
         <v>360</v>
       </c>
-      <c r="U131" s="23">
+      <c r="U131" s="24">
         <v>1.0</v>
       </c>
-      <c r="V131" s="27" t="s">
+      <c r="V131" s="25" t="s">
         <v>592</v>
       </c>
-    </row>
-    <row r="132" ht="15.75" hidden="1" customHeight="1">
+      <c r="W131" s="26"/>
+      <c r="X131" s="26"/>
+      <c r="Y131" s="26"/>
+      <c r="Z131" s="26"/>
+      <c r="AA131" s="26"/>
+      <c r="AB131" s="26"/>
+      <c r="AC131" s="26"/>
+      <c r="AD131" s="26"/>
+    </row>
+    <row r="132" ht="15.75" customHeight="1">
       <c r="A132" s="8">
         <v>2.155422499E9</v>
       </c>
@@ -36532,60 +36685,82 @@
       </c>
     </row>
     <row r="133" ht="15.75" customHeight="1">
-      <c r="A133" s="23">
+      <c r="A133" s="24">
         <v>3.309250332E9</v>
       </c>
-      <c r="B133" s="23" t="s">
+      <c r="B133" s="24" t="s">
         <v>593</v>
       </c>
-      <c r="C133" s="23" t="s">
+      <c r="C133" s="24" t="s">
         <v>427</v>
       </c>
-      <c r="D133" s="23">
+      <c r="D133" s="24">
         <v>2018.0</v>
       </c>
-      <c r="E133" s="23" t="s">
+      <c r="E133" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="F133" s="23" t="s">
+      <c r="F133" s="24" t="s">
         <v>594</v>
       </c>
-      <c r="G133" s="23" t="s">
+      <c r="G133" s="24" t="s">
         <v>595</v>
       </c>
-      <c r="H133" s="23" t="s">
+      <c r="H133" s="24" t="s">
         <v>596</v>
       </c>
-      <c r="I133" s="23" t="s">
+      <c r="I133" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="J133" s="23" t="s">
+      <c r="J133" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="K133" s="23" t="s">
+      <c r="K133" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="L133" s="23">
+      <c r="L133" s="24">
         <v>40.0</v>
       </c>
-      <c r="M133" s="10"/>
-      <c r="N133" s="10"/>
-      <c r="O133" s="10"/>
-      <c r="P133" s="10"/>
-      <c r="Q133" s="10"/>
-      <c r="R133" s="10"/>
-      <c r="S133" s="10"/>
-      <c r="T133" s="23" t="s">
+      <c r="M133" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="N133" s="25" t="s">
+        <v>683</v>
+      </c>
+      <c r="O133" s="25" t="s">
+        <v>678</v>
+      </c>
+      <c r="P133" s="25" t="s">
+        <v>679</v>
+      </c>
+      <c r="Q133" s="25" t="s">
+        <v>699</v>
+      </c>
+      <c r="R133" s="25" t="s">
+        <v>675</v>
+      </c>
+      <c r="S133" s="25" t="s">
+        <v>598</v>
+      </c>
+      <c r="T133" s="24" t="s">
         <v>360</v>
       </c>
-      <c r="U133" s="23">
+      <c r="U133" s="24">
         <v>1.0</v>
       </c>
-      <c r="V133" s="27" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="134" ht="15.75" hidden="1" customHeight="1">
+      <c r="V133" s="25" t="s">
+        <v>701</v>
+      </c>
+      <c r="W133" s="26"/>
+      <c r="X133" s="26"/>
+      <c r="Y133" s="26"/>
+      <c r="Z133" s="26"/>
+      <c r="AA133" s="26"/>
+      <c r="AB133" s="26"/>
+      <c r="AC133" s="26"/>
+      <c r="AD133" s="26"/>
+    </row>
+    <row r="134" ht="15.75" customHeight="1">
       <c r="A134" s="8">
         <v>3.309250332E9</v>
       </c>
@@ -36637,60 +36812,82 @@
       </c>
     </row>
     <row r="135" ht="15.75" customHeight="1">
-      <c r="A135" s="23">
+      <c r="A135" s="24">
         <v>3.625722965E9</v>
       </c>
-      <c r="B135" s="23" t="s">
+      <c r="B135" s="24" t="s">
         <v>600</v>
       </c>
-      <c r="C135" s="23" t="s">
+      <c r="C135" s="24" t="s">
         <v>601</v>
       </c>
-      <c r="D135" s="23">
+      <c r="D135" s="24">
         <v>2021.0</v>
       </c>
-      <c r="E135" s="23" t="s">
+      <c r="E135" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="F135" s="23" t="s">
+      <c r="F135" s="24" t="s">
         <v>602</v>
       </c>
-      <c r="G135" s="23" t="s">
+      <c r="G135" s="24" t="s">
         <v>603</v>
       </c>
-      <c r="H135" s="23" t="s">
+      <c r="H135" s="24" t="s">
         <v>604</v>
       </c>
-      <c r="I135" s="23" t="s">
+      <c r="I135" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="J135" s="23" t="s">
+      <c r="J135" s="24" t="s">
         <v>301</v>
       </c>
-      <c r="K135" s="23" t="s">
+      <c r="K135" s="24" t="s">
         <v>302</v>
       </c>
-      <c r="L135" s="23">
+      <c r="L135" s="24">
         <v>41.0</v>
       </c>
-      <c r="M135" s="10"/>
-      <c r="N135" s="10"/>
-      <c r="O135" s="10"/>
-      <c r="P135" s="10"/>
-      <c r="Q135" s="10"/>
-      <c r="R135" s="10"/>
-      <c r="S135" s="10"/>
-      <c r="T135" s="23" t="s">
+      <c r="M135" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="N135" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="O135" s="25" t="s">
+        <v>678</v>
+      </c>
+      <c r="P135" s="25" t="s">
+        <v>687</v>
+      </c>
+      <c r="Q135" s="25" t="s">
+        <v>699</v>
+      </c>
+      <c r="R135" s="25" t="s">
+        <v>689</v>
+      </c>
+      <c r="S135" s="25" t="s">
+        <v>607</v>
+      </c>
+      <c r="T135" s="24" t="s">
         <v>360</v>
       </c>
-      <c r="U135" s="23">
+      <c r="U135" s="24">
         <v>1.0</v>
       </c>
-      <c r="V135" s="27" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="136" ht="15.75" hidden="1" customHeight="1">
+      <c r="V135" s="25" t="s">
+        <v>702</v>
+      </c>
+      <c r="W135" s="26"/>
+      <c r="X135" s="26"/>
+      <c r="Y135" s="26"/>
+      <c r="Z135" s="26"/>
+      <c r="AA135" s="26"/>
+      <c r="AB135" s="26"/>
+      <c r="AC135" s="26"/>
+      <c r="AD135" s="26"/>
+    </row>
+    <row r="136" ht="15.75" customHeight="1">
       <c r="A136" s="8">
         <v>3.625722965E9</v>
       </c>
@@ -36742,68 +36939,82 @@
       </c>
     </row>
     <row r="137" ht="15.75" customHeight="1">
-      <c r="A137" s="23">
+      <c r="A137" s="24">
         <v>4.278392816E9</v>
       </c>
-      <c r="B137" s="23" t="s">
+      <c r="B137" s="24" t="s">
         <v>609</v>
       </c>
-      <c r="C137" s="23" t="s">
+      <c r="C137" s="24" t="s">
         <v>610</v>
       </c>
-      <c r="D137" s="23">
+      <c r="D137" s="24">
         <v>2019.0</v>
       </c>
-      <c r="E137" s="23" t="s">
+      <c r="E137" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="F137" s="23" t="s">
+      <c r="F137" s="24" t="s">
         <v>611</v>
       </c>
-      <c r="G137" s="23" t="s">
+      <c r="G137" s="24" t="s">
         <v>612</v>
       </c>
-      <c r="H137" s="23" t="s">
+      <c r="H137" s="24" t="s">
         <v>167</v>
       </c>
-      <c r="I137" s="23" t="s">
+      <c r="I137" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="J137" s="23" t="s">
+      <c r="J137" s="24" t="s">
         <v>613</v>
       </c>
-      <c r="K137" s="23" t="s">
+      <c r="K137" s="24" t="s">
         <v>614</v>
       </c>
-      <c r="L137" s="23">
+      <c r="L137" s="24">
         <v>42.0</v>
       </c>
-      <c r="M137" s="10"/>
-      <c r="N137" s="10"/>
-      <c r="O137" s="10"/>
-      <c r="P137" s="10"/>
-      <c r="Q137" s="10"/>
-      <c r="R137" s="10"/>
-      <c r="S137" s="10"/>
-      <c r="T137" s="23" t="s">
+      <c r="M137" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="N137" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="O137" s="25" t="s">
+        <v>686</v>
+      </c>
+      <c r="P137" s="25" t="s">
+        <v>687</v>
+      </c>
+      <c r="Q137" s="25" t="s">
+        <v>699</v>
+      </c>
+      <c r="R137" s="25" t="s">
+        <v>675</v>
+      </c>
+      <c r="S137" s="25" t="s">
+        <v>703</v>
+      </c>
+      <c r="T137" s="24" t="s">
         <v>360</v>
       </c>
-      <c r="U137" s="23">
+      <c r="U137" s="24">
         <v>1.0</v>
       </c>
       <c r="V137" s="27" t="s">
-        <v>618</v>
-      </c>
-      <c r="W137" s="23"/>
-      <c r="X137" s="23"/>
-      <c r="Y137" s="23"/>
-      <c r="Z137" s="23"/>
-      <c r="AA137" s="23"/>
-      <c r="AB137" s="23"/>
-      <c r="AC137" s="23"/>
-      <c r="AD137" s="23"/>
-    </row>
-    <row r="138" ht="15.75" hidden="1" customHeight="1">
+        <v>704</v>
+      </c>
+      <c r="W137" s="24"/>
+      <c r="X137" s="24"/>
+      <c r="Y137" s="24"/>
+      <c r="Z137" s="24"/>
+      <c r="AA137" s="24"/>
+      <c r="AB137" s="24"/>
+      <c r="AC137" s="24"/>
+      <c r="AD137" s="24"/>
+    </row>
+    <row r="138" ht="15.75" customHeight="1">
       <c r="A138" s="8">
         <v>4.278392816E9</v>
       </c>
@@ -36855,60 +37066,82 @@
       </c>
     </row>
     <row r="139" ht="15.75" customHeight="1">
-      <c r="A139" s="23">
+      <c r="A139" s="24">
         <v>5.66043228E8</v>
       </c>
-      <c r="B139" s="23" t="s">
+      <c r="B139" s="24" t="s">
         <v>619</v>
       </c>
-      <c r="C139" s="23" t="s">
+      <c r="C139" s="24" t="s">
         <v>620</v>
       </c>
-      <c r="D139" s="23">
+      <c r="D139" s="24">
         <v>2021.0</v>
       </c>
-      <c r="E139" s="23" t="s">
+      <c r="E139" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="F139" s="23" t="s">
+      <c r="F139" s="24" t="s">
         <v>147</v>
       </c>
-      <c r="G139" s="23" t="s">
+      <c r="G139" s="24" t="s">
         <v>621</v>
       </c>
-      <c r="H139" s="23" t="s">
+      <c r="H139" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="I139" s="23" t="s">
+      <c r="I139" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="J139" s="23" t="s">
+      <c r="J139" s="24" t="s">
         <v>622</v>
       </c>
-      <c r="K139" s="23" t="s">
+      <c r="K139" s="24" t="s">
         <v>623</v>
       </c>
-      <c r="L139" s="23">
+      <c r="L139" s="24">
         <v>43.0</v>
       </c>
-      <c r="M139" s="10"/>
-      <c r="N139" s="10"/>
-      <c r="O139" s="10"/>
-      <c r="P139" s="10"/>
-      <c r="Q139" s="10"/>
-      <c r="R139" s="10"/>
-      <c r="S139" s="10"/>
-      <c r="T139" s="23" t="s">
+      <c r="M139" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="N139" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="O139" s="25" t="s">
+        <v>686</v>
+      </c>
+      <c r="P139" s="25" t="s">
+        <v>679</v>
+      </c>
+      <c r="Q139" s="25" t="s">
+        <v>699</v>
+      </c>
+      <c r="R139" s="25" t="s">
+        <v>689</v>
+      </c>
+      <c r="S139" s="25" t="s">
+        <v>626</v>
+      </c>
+      <c r="T139" s="24" t="s">
         <v>360</v>
       </c>
-      <c r="U139" s="23">
+      <c r="U139" s="24">
         <v>1.0</v>
       </c>
-      <c r="V139" s="27" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="140" ht="15.75" hidden="1" customHeight="1">
+      <c r="V139" s="25" t="s">
+        <v>705</v>
+      </c>
+      <c r="W139" s="26"/>
+      <c r="X139" s="26"/>
+      <c r="Y139" s="26"/>
+      <c r="Z139" s="26"/>
+      <c r="AA139" s="26"/>
+      <c r="AB139" s="26"/>
+      <c r="AC139" s="26"/>
+      <c r="AD139" s="26"/>
+    </row>
+    <row r="140" ht="15.75" customHeight="1">
       <c r="A140" s="8">
         <v>5.66043228E8</v>
       </c>
@@ -36960,60 +37193,82 @@
       </c>
     </row>
     <row r="141" ht="15.75" customHeight="1">
-      <c r="A141" s="23">
+      <c r="A141" s="24">
         <v>8.53680639E8</v>
       </c>
-      <c r="B141" s="23" t="s">
+      <c r="B141" s="24" t="s">
         <v>628</v>
       </c>
-      <c r="C141" s="23" t="s">
+      <c r="C141" s="24" t="s">
         <v>629</v>
       </c>
-      <c r="D141" s="23">
+      <c r="D141" s="24">
         <v>2019.0</v>
       </c>
-      <c r="E141" s="23" t="s">
+      <c r="E141" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="F141" s="23" t="s">
+      <c r="F141" s="24" t="s">
         <v>630</v>
       </c>
-      <c r="G141" s="23" t="s">
+      <c r="G141" s="24" t="s">
         <v>631</v>
       </c>
-      <c r="H141" s="23" t="s">
+      <c r="H141" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="I141" s="23" t="s">
+      <c r="I141" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="J141" s="23" t="s">
+      <c r="J141" s="24" t="s">
         <v>183</v>
       </c>
-      <c r="K141" s="23" t="s">
+      <c r="K141" s="24" t="s">
         <v>184</v>
       </c>
-      <c r="L141" s="23">
+      <c r="L141" s="24">
         <v>44.0</v>
       </c>
-      <c r="M141" s="10"/>
-      <c r="N141" s="10"/>
-      <c r="O141" s="10"/>
-      <c r="P141" s="10"/>
-      <c r="Q141" s="10"/>
-      <c r="R141" s="10"/>
-      <c r="S141" s="10"/>
-      <c r="T141" s="23" t="s">
+      <c r="M141" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="N141" s="25" t="s">
+        <v>560</v>
+      </c>
+      <c r="O141" s="25" t="s">
+        <v>686</v>
+      </c>
+      <c r="P141" s="25" t="s">
+        <v>687</v>
+      </c>
+      <c r="Q141" s="25" t="s">
+        <v>699</v>
+      </c>
+      <c r="R141" s="25" t="s">
+        <v>689</v>
+      </c>
+      <c r="S141" s="25" t="s">
+        <v>635</v>
+      </c>
+      <c r="T141" s="24" t="s">
         <v>360</v>
       </c>
-      <c r="U141" s="23">
+      <c r="U141" s="24">
         <v>1.0</v>
       </c>
       <c r="V141" s="27" t="s">
-        <v>636</v>
-      </c>
-    </row>
-    <row r="142" ht="15.75" hidden="1" customHeight="1">
+        <v>706</v>
+      </c>
+      <c r="W141" s="26"/>
+      <c r="X141" s="26"/>
+      <c r="Y141" s="26"/>
+      <c r="Z141" s="26"/>
+      <c r="AA141" s="26"/>
+      <c r="AB141" s="26"/>
+      <c r="AC141" s="26"/>
+      <c r="AD141" s="26"/>
+    </row>
+    <row r="142" ht="15.75" customHeight="1">
       <c r="A142" s="8">
         <v>8.53680639E8</v>
       </c>
@@ -37065,60 +37320,82 @@
       </c>
     </row>
     <row r="143" ht="15.75" customHeight="1">
-      <c r="A143" s="23">
+      <c r="A143" s="24">
         <v>3.637456466E9</v>
       </c>
-      <c r="B143" s="23" t="s">
+      <c r="B143" s="24" t="s">
         <v>637</v>
       </c>
-      <c r="C143" s="23" t="s">
+      <c r="C143" s="24" t="s">
         <v>638</v>
       </c>
-      <c r="D143" s="23">
+      <c r="D143" s="24">
         <v>2020.0</v>
       </c>
-      <c r="E143" s="23" t="s">
+      <c r="E143" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="F143" s="23" t="s">
+      <c r="F143" s="24" t="s">
         <v>594</v>
       </c>
-      <c r="G143" s="23" t="s">
+      <c r="G143" s="24" t="s">
         <v>639</v>
       </c>
-      <c r="H143" s="23" t="s">
+      <c r="H143" s="24" t="s">
         <v>640</v>
       </c>
-      <c r="I143" s="23" t="s">
+      <c r="I143" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="J143" s="23" t="s">
+      <c r="J143" s="24" t="s">
         <v>641</v>
       </c>
-      <c r="K143" s="23" t="s">
+      <c r="K143" s="24" t="s">
         <v>642</v>
       </c>
-      <c r="L143" s="23">
+      <c r="L143" s="24">
         <v>45.0</v>
       </c>
-      <c r="M143" s="10"/>
-      <c r="N143" s="10"/>
-      <c r="O143" s="10"/>
-      <c r="P143" s="10"/>
-      <c r="Q143" s="10"/>
-      <c r="R143" s="10"/>
-      <c r="S143" s="10"/>
-      <c r="T143" s="23" t="s">
+      <c r="M143" s="25" t="s">
+        <v>707</v>
+      </c>
+      <c r="N143" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="O143" s="25" t="s">
+        <v>708</v>
+      </c>
+      <c r="P143" s="25" t="s">
+        <v>679</v>
+      </c>
+      <c r="Q143" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="R143" s="25" t="s">
+        <v>689</v>
+      </c>
+      <c r="S143" s="25" t="s">
+        <v>646</v>
+      </c>
+      <c r="T143" s="24" t="s">
         <v>360</v>
       </c>
-      <c r="U143" s="23">
+      <c r="U143" s="24">
         <v>1.0</v>
       </c>
-      <c r="V143" s="27" t="s">
-        <v>647</v>
-      </c>
-    </row>
-    <row r="144" ht="15.75" hidden="1" customHeight="1">
+      <c r="V143" s="25" t="s">
+        <v>709</v>
+      </c>
+      <c r="W143" s="26"/>
+      <c r="X143" s="26"/>
+      <c r="Y143" s="26"/>
+      <c r="Z143" s="26"/>
+      <c r="AA143" s="26"/>
+      <c r="AB143" s="26"/>
+      <c r="AC143" s="26"/>
+      <c r="AD143" s="26"/>
+    </row>
+    <row r="144" ht="15.75" customHeight="1">
       <c r="A144" s="8">
         <v>3.637456466E9</v>
       </c>
@@ -37170,60 +37447,82 @@
       </c>
     </row>
     <row r="145" ht="15.75" customHeight="1">
-      <c r="A145" s="23">
+      <c r="A145" s="24">
         <v>3.754172825E9</v>
       </c>
-      <c r="B145" s="23" t="s">
+      <c r="B145" s="24" t="s">
         <v>648</v>
       </c>
-      <c r="C145" s="23" t="s">
+      <c r="C145" s="24" t="s">
         <v>649</v>
       </c>
-      <c r="D145" s="23">
+      <c r="D145" s="24">
         <v>2022.0</v>
       </c>
-      <c r="E145" s="23" t="s">
+      <c r="E145" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="F145" s="23" t="s">
+      <c r="F145" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="G145" s="23" t="s">
+      <c r="G145" s="24" t="s">
         <v>650</v>
       </c>
-      <c r="H145" s="23" t="s">
+      <c r="H145" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="I145" s="23" t="s">
+      <c r="I145" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="J145" s="23" t="s">
+      <c r="J145" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="K145" s="23" t="s">
+      <c r="K145" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="L145" s="23">
+      <c r="L145" s="24">
         <v>46.0</v>
       </c>
-      <c r="M145" s="10"/>
-      <c r="N145" s="10"/>
-      <c r="O145" s="10"/>
-      <c r="P145" s="10"/>
-      <c r="Q145" s="10"/>
-      <c r="R145" s="10"/>
-      <c r="S145" s="10"/>
-      <c r="T145" s="23" t="s">
+      <c r="M145" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="N145" s="25" t="s">
+        <v>683</v>
+      </c>
+      <c r="O145" s="25" t="s">
+        <v>303</v>
+      </c>
+      <c r="P145" s="25" t="s">
+        <v>679</v>
+      </c>
+      <c r="Q145" s="25" t="s">
+        <v>680</v>
+      </c>
+      <c r="R145" s="25" t="s">
+        <v>689</v>
+      </c>
+      <c r="S145" s="25" t="s">
+        <v>654</v>
+      </c>
+      <c r="T145" s="24" t="s">
         <v>360</v>
       </c>
-      <c r="U145" s="23">
+      <c r="U145" s="24">
         <v>1.0</v>
       </c>
-      <c r="V145" s="27" t="s">
-        <v>655</v>
-      </c>
-    </row>
-    <row r="146" ht="15.75" hidden="1" customHeight="1">
+      <c r="V145" s="25" t="s">
+        <v>710</v>
+      </c>
+      <c r="W145" s="26"/>
+      <c r="X145" s="26"/>
+      <c r="Y145" s="26"/>
+      <c r="Z145" s="26"/>
+      <c r="AA145" s="26"/>
+      <c r="AB145" s="26"/>
+      <c r="AC145" s="26"/>
+      <c r="AD145" s="26"/>
+    </row>
+    <row r="146" ht="15.75" customHeight="1">
       <c r="A146" s="8">
         <v>3.754172825E9</v>
       </c>
@@ -37275,60 +37574,82 @@
       </c>
     </row>
     <row r="147" ht="15.75" customHeight="1">
-      <c r="A147" s="23">
+      <c r="A147" s="24">
         <v>1.296637108E9</v>
       </c>
-      <c r="B147" s="23" t="s">
+      <c r="B147" s="24" t="s">
         <v>656</v>
       </c>
-      <c r="C147" s="23" t="s">
+      <c r="C147" s="24" t="s">
         <v>657</v>
       </c>
-      <c r="D147" s="23">
+      <c r="D147" s="24">
         <v>2019.0</v>
       </c>
-      <c r="E147" s="23" t="s">
+      <c r="E147" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="F147" s="23" t="s">
+      <c r="F147" s="24" t="s">
         <v>658</v>
       </c>
-      <c r="G147" s="23" t="s">
+      <c r="G147" s="24" t="s">
         <v>659</v>
       </c>
-      <c r="H147" s="23" t="s">
+      <c r="H147" s="24" t="s">
         <v>192</v>
       </c>
-      <c r="I147" s="23" t="s">
+      <c r="I147" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="J147" s="23" t="s">
+      <c r="J147" s="24" t="s">
         <v>272</v>
       </c>
-      <c r="K147" s="23" t="s">
+      <c r="K147" s="24" t="s">
         <v>273</v>
       </c>
-      <c r="L147" s="23">
+      <c r="L147" s="24">
         <v>47.0</v>
       </c>
-      <c r="M147" s="10"/>
-      <c r="N147" s="10"/>
-      <c r="O147" s="10"/>
-      <c r="P147" s="10"/>
-      <c r="Q147" s="10"/>
-      <c r="R147" s="10"/>
-      <c r="S147" s="10"/>
-      <c r="T147" s="23" t="s">
+      <c r="M147" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="N147" s="25" t="s">
+        <v>560</v>
+      </c>
+      <c r="O147" s="25" t="s">
+        <v>303</v>
+      </c>
+      <c r="P147" s="25" t="s">
+        <v>687</v>
+      </c>
+      <c r="Q147" s="25" t="s">
+        <v>699</v>
+      </c>
+      <c r="R147" s="25" t="s">
+        <v>681</v>
+      </c>
+      <c r="S147" s="25" t="s">
+        <v>663</v>
+      </c>
+      <c r="T147" s="24" t="s">
         <v>360</v>
       </c>
-      <c r="U147" s="23">
+      <c r="U147" s="24">
         <v>1.0</v>
       </c>
       <c r="V147" s="27" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="148" ht="15.75" hidden="1" customHeight="1">
+        <v>711</v>
+      </c>
+      <c r="W147" s="26"/>
+      <c r="X147" s="26"/>
+      <c r="Y147" s="26"/>
+      <c r="Z147" s="26"/>
+      <c r="AA147" s="26"/>
+      <c r="AB147" s="26"/>
+      <c r="AC147" s="26"/>
+      <c r="AD147" s="26"/>
+    </row>
+    <row r="148" ht="15.75" customHeight="1">
       <c r="A148" s="8">
         <v>1.296637108E9</v>
       </c>
@@ -57852,18 +58173,7 @@
       <c r="V1001" s="23"/>
     </row>
   </sheetData>
-  <autoFilter ref="$A$1:$AD$148">
-    <filterColumn colId="20">
-      <filters blank="1">
-        <filter val="1"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="19">
-      <filters blank="1">
-        <filter val="Clayton"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="$A$1:$AD$148"/>
   <printOptions/>
   <pageMargins bottom="1.0" footer="0.0" header="0.0" left="0.75" right="0.75" top="1.0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>